<commit_message>
Added Gini to program
</commit_message>
<xml_diff>
--- a/PPPConverter/Sources/TempCalc.xlsx
+++ b/PPPConverter/Sources/TempCalc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\draco\source\repos\PPPConverter\PPPConverter\Sources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Draco\source\repos\dracoranger\PPPConverter\PPPConverter\Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D12E9C-8E60-4EDC-9CB9-215473180686}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4200A68-7F96-4945-B5B6-601F5C75081D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7CE1D539-8B48-47E8-809E-63922FA2B7F3}"/>
+    <workbookView xWindow="-21720" yWindow="-7875" windowWidth="21840" windowHeight="38040" xr2:uid="{7CE1D539-8B48-47E8-809E-63922FA2B7F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -571,304 +571,304 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>9.136819438494817E-2</c:v>
+                  <c:v>0.22725426539536592</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0123018855568098</c:v>
+                  <c:v>2.2098345349538397</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.5702468410261021</c:v>
+                  <c:v>9.248915561192387</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.852676785544599</c:v>
+                  <c:v>26.545068477857079</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>33.382353621737352</c:v>
+                  <c:v>61.282148323520637</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>69.244191571841625</c:v>
+                  <c:v>122.69152664328409</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>129.19409794817528</c:v>
+                  <c:v>222.10458127019851</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>222.75512899836212</c:v>
+                  <c:v>372.99728927806734</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>361.30413274484312</c:v>
+                  <c:v>591.02911194924661</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>558.15094029335182</c:v>
+                  <c:v>894.07754540449969</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>828.61153148568633</c:v>
+                  <c:v>1302.2692592878252</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1190.0762076557278</c:v>
+                  <c:v>1838.0084746147722</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1662.073546627124</c:v>
+                  <c:v>2526.0030584591782</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2266.3307384892814</c:v>
+                  <c:v>3393.2886968473686</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3026.8307751708035</c:v>
+                  <c:v>4469.2514261855613</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3969.8668749307885</c:v>
+                  <c:v>5785.6487452686151</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5124.0944539104385</c:v>
+                  <c:v>7376.6294868930145</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6520.5809040076774</c:v>
+                  <c:v>9278.7525956131813</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8192.8533950546807</c:v>
+                  <c:v>11531.004933178392</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>10176.944886534446</c:v>
+                  <c:v>14174.818213618759</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>12511.438507737834</c:v>
+                  <c:v>17254.085154405515</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>15237.510443819705</c:v>
+                  <c:v>20815.174917602722</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>18398.971447560205</c:v>
+                  <c:v>24906.947904744298</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>22042.30708196076</c:v>
+                  <c:v>29580.769960792721</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>26216.716786493089</c:v>
+                  <c:v>34890.526035578419</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>30974.151849408507</c:v>
+                  <c:v>40892.63334529155</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>36369.352359645309</c:v>
+                  <c:v>47646.054071678496</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>42459.883204265279</c:v>
+                  <c:v>55212.307632413271</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>49306.169170785353</c:v>
+                  <c:v>63655.482552534566</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>56971.529208072345</c:v>
+                  <c:v>73042.24796375788</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>65522.209894496977</c:v>
+                  <c:v>83441.86475580401</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>75027.418157683918</c:v>
+                  <c:v>94926.196401563095</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>85559.353286354177</c:v>
+                  <c:v>107569.71947588291</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>97193.238271359427</c:v>
+                  <c:v>121449.53388598622</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>110007.35050999073</c:v>
+                  <c:v>136645.37282994849</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>124083.05190495454</c:v>
+                  <c:v>153239.61249827346</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>139504.81838700283</c:v>
+                  <c:v>171317.28153236542</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>156360.26888804487</c:v>
+                  <c:v>190966.07025259157</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>174740.19378962374</c:v>
+                  <c:v>212276.33966763946</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>194738.58286988511</c:v>
+                  <c:v>235341.13027598604</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>216452.65277057665</c:v>
+                  <c:v>260256.1706694958</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>239982.87400417234</c:v>
+                  <c:v>287119.88594844338</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>265432.99751990376</c:v>
+                  <c:v>316033.40595660347</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>292910.08084628149</c:v>
+                  <c:v>347100.57334445661</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>322524.51382659416</c:v>
+                  <c:v>380427.95146802143</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>354390.04396286962</c:v>
+                  <c:v>416124.83213033114</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>388623.80138286005</c:v>
+                  <c:v>454303.24317212345</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>425346.3234437668</c:v>
+                  <c:v>495077.95591790136</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>464681.57898563659</c:v>
+                  <c:v>538566.49248314463</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>506756.99224664236</c:v>
+                  <c:v>584889.13294810569</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>551703.46645179205</c:v>
+                  <c:v>634168.92240330332</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>599655.40708599263</c:v>
+                  <c:v>686531.67787153402</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>650750.74486182223</c:v>
+                  <c:v>742105.99511094741</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>705130.95839182939</c:v>
+                  <c:v>801023.25530348171</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>762941.09657468577</c:v>
+                  <c:v>863417.63163272128</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>824329.80070405151</c:v>
+                  <c:v>929426.09575501992</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>889449.3263085864</c:v>
+                  <c:v>999188.42416753643</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>958455.56473113445</c:v>
+                  <c:v>1072847.2044766375</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1031508.064454732</c:v>
+                  <c:v>1150547.8415699496</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1108770.0521827384</c:v>
+                  <c:v>1232438.56369518</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1190408.4536800578</c:v>
+                  <c:v>1318670.4284486733</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>1276593.9143821052</c:v>
+                  <c:v>1409397.3286765276</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>1367500.8197778864</c:v>
+                  <c:v>1504775.9982909623</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>1463307.3155732777</c:v>
+                  <c:v>1604966.0180045031</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1564195.3276403393</c:v>
+                  <c:v>1710129.8209844339</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>1670350.5817582505</c:v>
+                  <c:v>1820432.6984298527</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>1781962.6231512232</c:v>
+                  <c:v>1936042.8050735693</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>1899224.8358285355</c:v>
+                  <c:v>2057131.1646109801</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>2022334.4617316213</c:v>
+                  <c:v>2183871.6750579672</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>2151492.6196929584</c:v>
+                  <c:v>2316441.1140397815</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>2286904.3242113097</c:v>
+                  <c:v>2455019.1440127846</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>2428778.5040477063</c:v>
+                  <c:v>2599788.3174208566</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>2577328.0206463854</c:v>
+                  <c:v>2750934.0817881855</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>2732769.6863847524</c:v>
+                  <c:v>2908644.78475011</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>2895324.2826562705</c:v>
+                  <c:v>3073111.6790235983</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>3065216.5777900619</c:v>
+                  <c:v>3244528.9273188985</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>3242675.3448108472</c:v>
+                  <c:v>3423093.6071938328</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>3427933.3790427363</c:v>
+                  <c:v>3609005.7158521502</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>3621227.5155602652</c:v>
+                  <c:v>3802468.1748873033</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>3822798.6464899378</c:v>
+                  <c:v>4003686.8349729585</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>4032891.7381654442</c:v>
+                  <c:v>4212870.4805015139</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>4251755.8481396036</c:v>
+                  <c:v>4430230.8341718307</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>4479644.1420559939</c:v>
+                  <c:v>4655982.5615273686</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>4716813.9103831174</c:v>
+                  <c:v>4890343.2754458496</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>4963526.5850138776</c:v>
+                  <c:v>5133533.5405815588</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>5220047.7557330336</c:v>
+                  <c:v>5385776.8777613202</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>5486647.186555244</c:v>
+                  <c:v>5647299.7683351962</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>5763598.8319361946</c:v>
+                  <c:v>5918331.6584828747</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>6051180.8528592549</c:v>
+                  <c:v>6199104.9634767128</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>6349675.6328000305</c:v>
+                  <c:v>6489855.0719023636</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>6659369.7935710931</c:v>
+                  <c:v>6790820.3498378675</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>6980554.2110491162</c:v>
+                  <c:v>7102242.1449920889</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>7313524.0307865748</c:v>
+                  <c:v>7424364.7908033235</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>7658578.6835101005</c:v>
+                  <c:v>7757435.6104989015</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>8016021.9005075376</c:v>
+                  <c:v>8101704.9211165607</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>8386161.7289056601</c:v>
+                  <c:v>8457426.0374883655</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>8769310.5468404852</c:v>
+                  <c:v>8824855.2761878967</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>9165785.0785220526</c:v>
+                  <c:v>9204251.9594414458</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>9575906.4091954678</c:v>
+                  <c:v>9595878.419003902</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>10000000.000000006</c:v>
+                  <c:v>10000000.000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1961,14 +1961,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D864C3B-E825-406D-92B0-B90D1A840648}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="34.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2128,123 +2129,251 @@
       <c r="A6" t="s">
         <v>11</v>
       </c>
+      <c r="B6">
+        <f>B2*B7</f>
+        <v>0.51990000000000003</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:I6" si="2">C2*C7</f>
+        <v>5.3750000000000006E-2</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="2"/>
+        <v>0.15537500000000001</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>8.2475000000000021E-2</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>8.9249999999999996E-2</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>7.7550000000000008E-2</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="2"/>
+        <v>3.0175E-2</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>3.0525000000000004E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7">
-        <f>B5*0.75</f>
-        <v>3.7615740740740744</v>
+        <f>B5-(1/4*($B$5-$B$13))</f>
+        <v>4.0115740740740744</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:I7" si="2">C5*0.75</f>
-        <v>0.57692307692307698</v>
+        <f>C5+(1/4*(C$13-C$5))</f>
+        <v>0.82692307692307698</v>
       </c>
       <c r="D7">
-        <f t="shared" si="2"/>
-        <v>0.23328149300155521</v>
+        <f>D5+(1/4*(D$13-D$5))</f>
+        <v>0.48328149300155521</v>
       </c>
       <c r="E7">
-        <f t="shared" si="2"/>
-        <v>2.5083612040133785</v>
+        <f>E5-(1/4*($E$5-$E$13))</f>
+        <v>2.7583612040133785</v>
       </c>
       <c r="F7">
-        <f t="shared" si="2"/>
-        <v>0.1811594202898551</v>
+        <f>F5+(1/4*(F$13-F$5))</f>
+        <v>0.4311594202898551</v>
       </c>
       <c r="G7">
-        <f t="shared" si="2"/>
-        <v>7.3529411764705888</v>
+        <f>G5-(1/4*($G$5-$G$13))</f>
+        <v>7.6029411764705888</v>
       </c>
       <c r="H7">
-        <f t="shared" si="2"/>
-        <v>6.37213254035684E-3</v>
+        <f>H5+(1/4*(H$13-H$5))</f>
+        <v>0.25637213254035685</v>
       </c>
       <c r="I7">
-        <f t="shared" si="2"/>
-        <v>6.2972292191435762E-3</v>
+        <f>I5+(1/4*(I$13-I$5))</f>
+        <v>0.25629722921914361</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
+      <c r="B8">
+        <f>B2*B9</f>
+        <v>0.38979999999999998</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:I8" si="3">C2*C9</f>
+        <v>5.7500000000000009E-2</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="3"/>
+        <v>0.21074999999999999</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="3"/>
+        <v>6.4950000000000022E-2</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="3"/>
+        <v>0.1285</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="3"/>
+        <v>5.510000000000001E-2</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="3"/>
+        <v>5.9350000000000007E-2</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>6.0049999999999999E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9">
-        <f>0.5*B5</f>
-        <v>2.5077160493827164</v>
+        <f t="shared" ref="B8:B11" si="4">B7-(1/4*($B$5-$B$13))</f>
+        <v>3.007716049382716</v>
       </c>
       <c r="C9">
-        <f t="shared" ref="C9:I9" si="3">0.5*C5</f>
-        <v>0.38461538461538464</v>
+        <f t="shared" ref="C8:D11" si="5">C7+(1/4*(C$13-C$5))</f>
+        <v>0.88461538461538469</v>
       </c>
       <c r="D9">
-        <f t="shared" si="3"/>
-        <v>0.15552099533437014</v>
+        <f t="shared" si="5"/>
+        <v>0.65552099533437014</v>
       </c>
       <c r="E9">
-        <f t="shared" si="3"/>
-        <v>1.6722408026755855</v>
+        <f t="shared" ref="E8:E11" si="6">E7-(1/4*($E$5-$E$13))</f>
+        <v>2.1722408026755859</v>
       </c>
       <c r="F9">
-        <f t="shared" si="3"/>
-        <v>0.12077294685990339</v>
+        <f t="shared" ref="F8:F11" si="7">F7+(1/4*(F$13-F$5))</f>
+        <v>0.62077294685990347</v>
       </c>
       <c r="G9">
-        <f t="shared" si="3"/>
-        <v>4.9019607843137258</v>
+        <f t="shared" ref="G8:G11" si="8">G7-(1/4*($G$5-$G$13))</f>
+        <v>5.4019607843137258</v>
       </c>
       <c r="H9">
-        <f t="shared" si="3"/>
-        <v>4.248088360237893E-3</v>
+        <f t="shared" ref="H9:I9" si="9">H7+(1/4*(H$13-H$5))</f>
+        <v>0.50424808836023793</v>
       </c>
       <c r="I9">
-        <f t="shared" si="3"/>
-        <v>4.1981528127623844E-3</v>
+        <f t="shared" si="9"/>
+        <v>0.50419815281276237</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
+      <c r="B10">
+        <f>B2*B11</f>
+        <v>0.25969999999999993</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ref="C10:I10" si="10">C2*C11</f>
+        <v>6.1250000000000006E-2</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="10"/>
+        <v>0.266125</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="10"/>
+        <v>4.7425000000000016E-2</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="10"/>
+        <v>0.16775000000000001</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="10"/>
+        <v>3.2650000000000005E-2</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="10"/>
+        <v>8.8525000000000006E-2</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="10"/>
+        <v>8.9575000000000002E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11">
-        <f>0.25*B5</f>
-        <v>1.2538580246913582</v>
+        <f t="shared" si="4"/>
+        <v>2.0038580246913575</v>
       </c>
       <c r="C11">
-        <f t="shared" ref="C11:I11" si="4">0.25*C5</f>
-        <v>0.19230769230769232</v>
+        <f t="shared" si="5"/>
+        <v>0.9423076923076924</v>
       </c>
       <c r="D11">
-        <f t="shared" si="4"/>
-        <v>7.7760497667185069E-2</v>
+        <f t="shared" si="5"/>
+        <v>0.82776049766718507</v>
       </c>
       <c r="E11">
-        <f t="shared" si="4"/>
-        <v>0.83612040133779275</v>
+        <f t="shared" si="6"/>
+        <v>1.5861204013377932</v>
       </c>
       <c r="F11">
-        <f t="shared" si="4"/>
-        <v>6.0386473429951695E-2</v>
+        <f t="shared" si="7"/>
+        <v>0.81038647342995174</v>
       </c>
       <c r="G11">
-        <f t="shared" si="4"/>
-        <v>2.4509803921568629</v>
+        <f t="shared" si="8"/>
+        <v>3.2009803921568629</v>
       </c>
       <c r="H11">
-        <f t="shared" si="4"/>
-        <v>2.1240441801189465E-3</v>
+        <f t="shared" ref="H11:I11" si="11">H9+(1/4*(H$13-H$5))</f>
+        <v>0.75212404418011902</v>
       </c>
       <c r="I11">
-        <f t="shared" si="4"/>
-        <v>2.0990764063811922E-3</v>
+        <f t="shared" si="11"/>
+        <v>0.75209907640638118</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
+      <c r="B12">
+        <f>B2*B13</f>
+        <v>0.12959999999999999</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:I12" si="12">C2*C13</f>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="12"/>
+        <v>0.32150000000000001</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="12"/>
+        <v>2.9899999999999999E-2</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="12"/>
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="12"/>
+        <v>1.0200000000000001E-2</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="12"/>
+        <v>0.1177</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="12"/>
+        <v>0.1191</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13">
@@ -2276,13 +2405,105 @@
       <c r="A14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <f>B2*B15</f>
+        <v>-5.0000000000002375E-4</v>
+      </c>
+      <c r="C14">
+        <f>C2*C15</f>
+        <v>6.8750000000000006E-2</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14:F14" si="13">D2*D15</f>
+        <v>0.37687500000000002</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="13"/>
+        <v>1.2374999999999997E-2</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="13"/>
+        <v>0.24624999999999997</v>
+      </c>
+      <c r="G14">
+        <f>G2*G15</f>
+        <v>-1.2250000000000002E-2</v>
+      </c>
+      <c r="H14">
+        <f t="shared" ref="H14" si="14">H2*H15</f>
+        <v>0.14687500000000001</v>
+      </c>
+      <c r="I14">
+        <f t="shared" ref="I14" si="15">I2*I15</f>
+        <v>0.14862500000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <f>B13-(1/4*($B$5-$B$13))</f>
+        <v>-3.8580246913582084E-3</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:D15" si="16">C13+(1/4*(C$13-C$5))</f>
+        <v>1.0576923076923077</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="16"/>
+        <v>1.1722395023328149</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ref="E15" si="17">E13-(1/4*($E$5-$E$13))</f>
+        <v>0.41387959866220725</v>
+      </c>
+      <c r="F15">
+        <f t="shared" ref="F15" si="18">F13+(1/4*(F$13-F$5))</f>
+        <v>1.1896135265700483</v>
+      </c>
+      <c r="G15">
+        <f t="shared" ref="G15" si="19">G13-(1/4*($G$5-$G$13))</f>
+        <v>-1.2009803921568629</v>
+      </c>
+      <c r="H15">
+        <f t="shared" ref="H15:I15" si="20">H13+(1/4*(H$13-H$5))</f>
+        <v>1.2478759558198811</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="20"/>
+        <v>1.2479009235936189</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
       <c r="B20">
         <v>0.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>0.13</v>
+      </c>
+      <c r="C24">
+        <v>6.8750000000000006E-2</v>
+      </c>
+      <c r="D24">
+        <v>0.3</v>
+      </c>
+      <c r="E24">
+        <v>1.2375000000000001E-2</v>
+      </c>
+      <c r="F24">
+        <v>0.20624999999999999</v>
+      </c>
+      <c r="G24">
+        <v>0.01</v>
+      </c>
+      <c r="H24">
+        <v>0.12687499999999999</v>
+      </c>
+      <c r="I24">
+        <v>0.14862500000000001</v>
       </c>
     </row>
   </sheetData>
@@ -2295,7 +2516,7 @@
   <dimension ref="A1:K101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2328,7 +2549,7 @@
         <v>15</v>
       </c>
       <c r="I1">
-        <v>0.7</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2336,15 +2557,16 @@
         <v>1</v>
       </c>
       <c r="B2">
+        <f>A2^(1/(1-$I$1))</f>
         <v>1</v>
       </c>
       <c r="C2">
         <f>B2/SUM(B:B)*$I$5</f>
-        <v>9.136819438494817E-2</v>
+        <v>0.22725426539536592</v>
       </c>
       <c r="D2">
         <f>C2</f>
-        <v>9.136819438494817E-2</v>
+        <v>0.22725426539536592</v>
       </c>
       <c r="E2">
         <f>B2</f>
@@ -2371,30 +2593,30 @@
       </c>
       <c r="B3">
         <f>A3^(1/(1-$I$1))</f>
-        <v>10.07936839915898</v>
+        <v>8.7240618613220615</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C66" si="0">B3/SUM($B$2:$B$101)*$I$5</f>
-        <v>0.92093369117186152</v>
+        <f t="shared" ref="C3:C66" si="0">B3/SUM(B:B)*$I$5</f>
+        <v>1.9825802695584738</v>
       </c>
       <c r="D3">
         <f>D2+C3</f>
-        <v>1.0123018855568098</v>
+        <v>2.2098345349538397</v>
       </c>
       <c r="E3">
         <f>E2+B3</f>
-        <v>11.07936839915898</v>
+        <v>9.7240618613220615</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F66" si="1">A3*B3</f>
-        <v>20.15873679831796</v>
+        <v>17.448123722644123</v>
       </c>
       <c r="H3" t="s">
         <v>16</v>
       </c>
       <c r="I3">
         <f>2*SUM(F:F)</f>
-        <v>17873469224.551502</v>
+        <v>7118677460.5709496</v>
       </c>
       <c r="J3">
         <f>(I2+1)/I2</f>
@@ -2402,7 +2624,7 @@
       </c>
       <c r="K3">
         <f>I3/I4-J3</f>
-        <v>0.62306661044221046</v>
+        <v>0.60774981688859997</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2411,27 +2633,27 @@
       </c>
       <c r="B4">
         <f t="shared" ref="B4:B67" si="2">A4^(1/(1-$I$1))</f>
-        <v>38.940738398300034</v>
+        <v>30.974472641876702</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>3.5579449554692926</v>
+        <v>7.0390810262385477</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D67" si="3">D3+C4</f>
-        <v>4.5702468410261021</v>
+        <v>9.248915561192387</v>
       </c>
       <c r="E4">
         <f t="shared" ref="E4:E67" si="4">E3+B4</f>
-        <v>50.020106797459015</v>
+        <v>40.698534503198765</v>
       </c>
       <c r="F4">
         <f t="shared" si="1"/>
-        <v>116.82221519490011</v>
+        <v>92.923417925630105</v>
       </c>
       <c r="I4">
         <f>I2*SUM(B:B)</f>
-        <v>10944727612.618097</v>
+        <v>4400357450.9822674</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -2440,23 +2662,23 @@
       </c>
       <c r="B5">
         <f t="shared" si="2"/>
-        <v>101.59366732596467</v>
+        <v>76.10925536017416</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>9.2824299445184977</v>
+        <v>17.296152916664692</v>
       </c>
       <c r="D5">
         <f t="shared" si="3"/>
-        <v>13.852676785544599</v>
+        <v>26.545068477857079</v>
       </c>
       <c r="E5">
         <f t="shared" si="4"/>
-        <v>151.6137741234237</v>
+        <v>116.80778986337293</v>
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
-        <v>406.3746693038587</v>
+        <v>304.43702144069664</v>
       </c>
       <c r="H5" t="s">
         <v>24</v>
@@ -2471,23 +2693,23 @@
       </c>
       <c r="B6">
         <f t="shared" si="2"/>
-        <v>213.7469933345869</v>
+        <v>152.85556812423158</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>19.529676836192756</v>
+        <v>34.737079845663558</v>
       </c>
       <c r="D6">
         <f t="shared" si="3"/>
-        <v>33.382353621737352</v>
+        <v>61.282148323520637</v>
       </c>
       <c r="E6">
         <f t="shared" si="4"/>
-        <v>365.36076745801063</v>
+        <v>269.66335798760451</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
-        <v>1068.7349666729344</v>
+        <v>764.27784062115791</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -2496,23 +2718,23 @@
       </c>
       <c r="B7">
         <f t="shared" si="2"/>
-        <v>392.49804805174188</v>
+        <v>270.22321544956003</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>35.861837950104274</v>
+        <v>61.409378319763455</v>
       </c>
       <c r="D7">
         <f t="shared" si="3"/>
-        <v>69.244191571841625</v>
+        <v>122.69152664328409</v>
       </c>
       <c r="E7">
         <f t="shared" si="4"/>
-        <v>757.8588155097525</v>
+        <v>539.88657343716454</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>2354.988288310451</v>
+        <v>1621.3392926973602</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2521,23 +2743,23 @@
       </c>
       <c r="B8">
         <f t="shared" si="2"/>
-        <v>656.13539569092882</v>
+        <v>437.45297565245005</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>59.949906376333665</v>
+        <v>99.413054626914416</v>
       </c>
       <c r="D8">
         <f t="shared" si="3"/>
-        <v>129.19409794817528</v>
+        <v>222.10458127019851</v>
       </c>
       <c r="E8">
         <f t="shared" si="4"/>
-        <v>1413.9942112006813</v>
+        <v>977.33954908961459</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>4592.9477698365017</v>
+        <v>3062.1708295671506</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -2546,23 +2768,23 @@
       </c>
       <c r="B9">
         <f t="shared" si="2"/>
-        <v>1023.9999999999991</v>
+        <v>663.98185198131739</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>93.561031050186841</v>
+        <v>150.89270800786886</v>
       </c>
       <c r="D9">
         <f t="shared" si="3"/>
-        <v>222.75512899836212</v>
+        <v>372.99728927806734</v>
       </c>
       <c r="E9">
         <f t="shared" si="4"/>
-        <v>2437.9942112006802</v>
+        <v>1641.3214010709321</v>
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>8191.9999999999927</v>
+        <v>5311.8548158505391</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2571,23 +2793,23 @@
       </c>
       <c r="B10">
         <f t="shared" si="2"/>
-        <v>1516.3811070048387</v>
+        <v>959.41795544236822</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>138.54900374648099</v>
+        <v>218.03182267117927</v>
       </c>
       <c r="D10">
         <f t="shared" si="3"/>
-        <v>361.30413274484312</v>
+        <v>591.02911194924661</v>
       </c>
       <c r="E10">
         <f t="shared" si="4"/>
-        <v>3954.3753182055189</v>
+        <v>2600.7393565133002</v>
       </c>
       <c r="F10">
         <f t="shared" si="1"/>
-        <v>13647.429963043549</v>
+        <v>8634.7615989813148</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -2596,23 +2818,23 @@
       </c>
       <c r="B11">
         <f t="shared" si="2"/>
-        <v>2154.4346900318833</v>
+        <v>1333.5214321633268</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>196.84680754850868</v>
+        <v>303.04843345525313</v>
       </c>
       <c r="D11">
         <f t="shared" si="3"/>
-        <v>558.15094029335182</v>
+        <v>894.07754540449969</v>
       </c>
       <c r="E11">
         <f t="shared" si="4"/>
-        <v>6108.8100082374021</v>
+        <v>3934.2607886766273</v>
       </c>
       <c r="F11">
         <f t="shared" si="1"/>
-        <v>21544.346900318833</v>
+        <v>13335.214321633268</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -2621,23 +2843,23 @@
       </c>
       <c r="B12">
         <f t="shared" si="2"/>
-        <v>2960.1175005477585</v>
+        <v>1796.1894496157126</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>270.4605911923345</v>
+        <v>408.19171388332541</v>
       </c>
       <c r="D12">
         <f t="shared" si="3"/>
-        <v>828.61153148568633</v>
+        <v>1302.2692592878252</v>
       </c>
       <c r="E12">
         <f t="shared" si="4"/>
-        <v>9068.9275087851602</v>
+        <v>5730.4502382923401</v>
       </c>
       <c r="F12">
         <f t="shared" si="1"/>
-        <v>32561.292506025344</v>
+        <v>19758.08394577284</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2646,23 +2868,23 @@
       </c>
       <c r="B13">
         <f t="shared" si="2"/>
-        <v>3956.132422264312</v>
+        <v>2357.4440479473242</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>361.46467617004151</v>
+        <v>535.73921532694692</v>
       </c>
       <c r="D13">
         <f t="shared" si="3"/>
-        <v>1190.0762076557278</v>
+        <v>1838.0084746147722</v>
       </c>
       <c r="E13">
         <f t="shared" si="4"/>
-        <v>13025.059931049473</v>
+        <v>8087.8942862396643</v>
       </c>
       <c r="F13">
         <f t="shared" si="1"/>
-        <v>47473.589067171742</v>
+        <v>28289.32857536789</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -2671,23 +2893,23 @@
       </c>
       <c r="B14">
         <f t="shared" si="2"/>
-        <v>5165.8823089225025</v>
+        <v>3027.4220932551757</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>471.99733897139606</v>
+        <v>687.99458384440584</v>
       </c>
       <c r="D14">
         <f t="shared" si="3"/>
-        <v>1662.073546627124</v>
+        <v>2526.0030584591782</v>
       </c>
       <c r="E14">
         <f t="shared" si="4"/>
-        <v>18190.942239971977</v>
+        <v>11115.31637949484</v>
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>67156.470015992527</v>
+        <v>39356.487212317283</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -2696,23 +2918,23 @@
       </c>
       <c r="B15">
         <f t="shared" si="2"/>
-        <v>6613.4303728968243</v>
+        <v>3816.366821011386</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>604.25719186215724</v>
+        <v>867.28563838819048</v>
       </c>
       <c r="D15">
         <f t="shared" si="3"/>
-        <v>2266.3307384892814</v>
+        <v>3393.2886968473686</v>
       </c>
       <c r="E15">
         <f t="shared" si="4"/>
-        <v>24804.372612868799</v>
+        <v>14931.683200506226</v>
       </c>
       <c r="F15">
         <f t="shared" si="1"/>
-        <v>92588.025220555544</v>
+        <v>53429.135494159404</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -2721,23 +2943,23 @@
       </c>
       <c r="B16">
         <f t="shared" si="2"/>
-        <v>8323.465750865329</v>
+        <v>4734.6206130225319</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>760.50003668152181</v>
+        <v>1075.9627293381925</v>
       </c>
       <c r="D16">
         <f t="shared" si="3"/>
-        <v>3026.8307751708035</v>
+        <v>4469.2514261855613</v>
       </c>
       <c r="E16">
         <f t="shared" si="4"/>
-        <v>33127.838363734132</v>
+        <v>19666.303813528757</v>
       </c>
       <c r="F16">
         <f t="shared" si="1"/>
-        <v>124851.98626297993</v>
+        <v>71019.309195337977</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -2746,23 +2968,23 @@
       </c>
       <c r="B17">
         <f t="shared" si="2"/>
-        <v>10321.273240738783</v>
+        <v>5792.6187514801986</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>943.03609975998495</v>
+        <v>1316.3973190830541</v>
       </c>
       <c r="D17">
         <f t="shared" si="3"/>
-        <v>3969.8668749307885</v>
+        <v>5785.6487452686151</v>
       </c>
       <c r="E17">
         <f t="shared" si="4"/>
-        <v>43449.111604472913</v>
+        <v>25458.922565008957</v>
       </c>
       <c r="F17">
         <f t="shared" si="1"/>
-        <v>165140.37185182053</v>
+        <v>92681.900023683178</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2771,23 +2993,23 @@
       </c>
       <c r="B18">
         <f t="shared" si="2"/>
-        <v>12632.706454903906</v>
+        <v>7000.8839607762184</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>1154.2275789796495</v>
+        <v>1590.9807416243991</v>
       </c>
       <c r="D18">
         <f t="shared" si="3"/>
-        <v>5124.0944539104385</v>
+        <v>7376.6294868930145</v>
       </c>
       <c r="E18">
         <f t="shared" si="4"/>
-        <v>56081.818059376819</v>
+        <v>32459.806525785178</v>
       </c>
       <c r="F18">
         <f t="shared" si="1"/>
-        <v>214756.0097333664</v>
+        <v>119015.02733319571</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -2796,23 +3018,23 @@
       </c>
       <c r="B19">
         <f t="shared" si="2"/>
-        <v>15284.163811026276</v>
+        <v>8370.021594142343</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>1396.4864500972387</v>
+        <v>1902.1231087201675</v>
       </c>
       <c r="D19">
         <f t="shared" si="3"/>
-        <v>6520.5809040076774</v>
+        <v>9278.7525956131813</v>
       </c>
       <c r="E19">
         <f t="shared" si="4"/>
-        <v>71365.981870403091</v>
+        <v>40829.828119927522</v>
       </c>
       <c r="F19">
         <f t="shared" si="1"/>
-        <v>275114.94859847298</v>
+        <v>150660.38869456216</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2821,23 +3043,23 @@
       </c>
       <c r="B20">
         <f t="shared" si="2"/>
-        <v>18302.566908583787</v>
+        <v>9910.7153550973089</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>1672.2724910470031</v>
+        <v>2252.2523375652117</v>
       </c>
       <c r="D20">
         <f t="shared" si="3"/>
-        <v>8192.8533950546807</v>
+        <v>11531.004933178392</v>
       </c>
       <c r="E20">
         <f t="shared" si="4"/>
-        <v>89668.548778986878</v>
+        <v>50740.543475024831</v>
       </c>
       <c r="F20">
         <f t="shared" si="1"/>
-        <v>347748.77126309194</v>
+        <v>188303.59174684886</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2846,23 +3068,23 @@
       </c>
       <c r="B21">
         <f t="shared" si="2"/>
-        <v>21715.340932759209</v>
+        <v>11633.723467591639</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>1984.091491479765</v>
+        <v>2643.8132804403667</v>
       </c>
       <c r="D21">
         <f t="shared" si="3"/>
-        <v>10176.944886534446</v>
+        <v>14174.818213618759</v>
       </c>
       <c r="E21">
         <f t="shared" si="4"/>
-        <v>111383.88971174609</v>
+        <v>62374.266942616472</v>
       </c>
       <c r="F21">
         <f t="shared" si="1"/>
-        <v>434306.81865518418</v>
+        <v>232674.46935183278</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2871,23 +3093,23 @@
       </c>
       <c r="B22">
         <f t="shared" si="2"/>
-        <v>25550.396797465539</v>
+        <v>13549.875226454369</v>
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>2334.4936212033886</v>
+        <v>3079.2669407867547</v>
       </c>
       <c r="D22">
         <f t="shared" si="3"/>
-        <v>12511.438507737834</v>
+        <v>17254.085154405515</v>
       </c>
       <c r="E22">
         <f t="shared" si="4"/>
-        <v>136934.28650921164</v>
+        <v>75924.142169070838</v>
       </c>
       <c r="F22">
         <f t="shared" si="1"/>
-        <v>536558.33274677629</v>
+        <v>284547.37975554174</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2896,23 +3118,23 @@
       </c>
       <c r="B23">
         <f t="shared" si="2"/>
-        <v>29836.114792818531</v>
+        <v>15670.06787310151</v>
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>2726.0719360818712</v>
+        <v>3561.0897631972075</v>
       </c>
       <c r="D23">
         <f t="shared" si="3"/>
-        <v>15237.510443819705</v>
+        <v>20815.174917602722</v>
       </c>
       <c r="E23">
         <f t="shared" si="4"/>
-        <v>166770.40130203016</v>
+        <v>91594.210042172344</v>
       </c>
       <c r="F23">
         <f t="shared" si="1"/>
-        <v>656394.5254420077</v>
+        <v>344741.49320823321</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2921,23 +3143,23 @@
       </c>
       <c r="B24">
         <f t="shared" si="2"/>
-        <v>34601.329543853957</v>
+        <v>18005.263751696406</v>
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>3161.4610037404987</v>
+        <v>4091.7729871415768</v>
       </c>
       <c r="D24">
         <f t="shared" si="3"/>
-        <v>18398.971447560205</v>
+        <v>24906.947904744298</v>
       </c>
       <c r="E24">
         <f t="shared" si="4"/>
-        <v>201371.73084588413</v>
+        <v>109599.47379386875</v>
       </c>
       <c r="F24">
         <f t="shared" si="1"/>
-        <v>795830.57950864104</v>
+        <v>414121.06628901733</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2946,23 +3168,23 @@
       </c>
       <c r="B25">
         <f t="shared" si="2"/>
-        <v>39875.316119859235</v>
+        <v>20566.487708897941</v>
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>3643.3356344005556</v>
+        <v>4673.8220560484233</v>
       </c>
       <c r="D25">
         <f t="shared" si="3"/>
-        <v>22042.30708196076</v>
+        <v>29580.769960792721</v>
       </c>
       <c r="E25">
         <f t="shared" si="4"/>
-        <v>241247.04696574336</v>
+        <v>130165.96150276669</v>
       </c>
       <c r="F25">
         <f t="shared" si="1"/>
-        <v>957007.5868766217</v>
+        <v>493595.70501355059</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2971,23 +3193,23 @@
       </c>
       <c r="B26">
         <f t="shared" si="2"/>
-        <v>45687.777159575933</v>
+        <v>23364.824706581607</v>
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>4174.4097045323288</v>
+        <v>5309.7560747856987</v>
       </c>
       <c r="D26">
         <f t="shared" si="3"/>
-        <v>26216.716786493089</v>
+        <v>34890.526035578419</v>
       </c>
       <c r="E26">
         <f t="shared" si="4"/>
-        <v>286934.82412531931</v>
+        <v>153530.7862093483</v>
       </c>
       <c r="F26">
         <f t="shared" si="1"/>
-        <v>1142194.4289893983</v>
+        <v>584120.61766454019</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2996,23 +3218,23 @@
       </c>
       <c r="B27">
         <f t="shared" si="2"/>
-        <v>52068.830898327884</v>
+        <v>26411.417621891294</v>
       </c>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>4757.4350629154169</v>
+        <v>6002.1073097131275</v>
       </c>
       <c r="D27">
         <f t="shared" si="3"/>
-        <v>30974.151849408507</v>
+        <v>40892.63334529155</v>
       </c>
       <c r="E27">
         <f t="shared" si="4"/>
-        <v>339003.65502364718</v>
+        <v>179942.2038312396</v>
       </c>
       <c r="F27">
         <f t="shared" si="1"/>
-        <v>1353789.6033565251</v>
+        <v>686696.85816917371</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -3021,23 +3243,23 @@
       </c>
       <c r="B28">
         <f t="shared" si="2"/>
-        <v>59048.999999999978</v>
+        <v>29717.46521297489</v>
       </c>
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>5395.2005102368021</v>
+        <v>6753.4207263869494</v>
       </c>
       <c r="D28">
         <f t="shared" si="3"/>
-        <v>36369.352359645309</v>
+        <v>47646.054071678496</v>
       </c>
       <c r="E28">
         <f t="shared" si="4"/>
-        <v>398052.65502364718</v>
+        <v>209659.6690442145</v>
       </c>
       <c r="F28">
         <f t="shared" si="1"/>
-        <v>1594322.9999999993</v>
+        <v>802371.56075032207</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -3046,23 +3268,23 @@
       </c>
       <c r="B29">
         <f t="shared" si="2"/>
-        <v>66659.20111061442</v>
+        <v>33294.220232000371</v>
       </c>
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>6090.5308446199706</v>
+        <v>7566.2535607347727</v>
       </c>
       <c r="D29">
         <f t="shared" si="3"/>
-        <v>42459.883204265279</v>
+        <v>55212.307632413271</v>
       </c>
       <c r="E29">
         <f t="shared" si="4"/>
-        <v>464711.85613426159</v>
+        <v>242953.88927621488</v>
       </c>
       <c r="F29">
         <f t="shared" si="1"/>
-        <v>1866457.6310972038</v>
+        <v>932238.16649601038</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -3071,23 +3293,23 @@
       </c>
       <c r="B30">
         <f t="shared" si="2"/>
-        <v>74930.735061652042</v>
+        <v>37152.987669702343</v>
       </c>
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>6846.2859665200749</v>
+        <v>8443.1749201212933</v>
       </c>
       <c r="D30">
         <f t="shared" si="3"/>
-        <v>49306.169170785353</v>
+        <v>63655.482552534566</v>
       </c>
       <c r="E30">
         <f t="shared" si="4"/>
-        <v>539642.59119591361</v>
+        <v>280106.8769459172</v>
       </c>
       <c r="F30">
         <f t="shared" si="1"/>
-        <v>2172991.3167879093</v>
+        <v>1077436.642421368</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -3096,23 +3318,23 @@
       </c>
       <c r="B31">
         <f t="shared" si="2"/>
-        <v>83895.277660754189</v>
+        <v>41305.123117899166</v>
       </c>
       <c r="C31">
         <f t="shared" si="0"/>
-        <v>7665.3600372869887</v>
+        <v>9386.7654112233195</v>
       </c>
       <c r="D31">
         <f t="shared" si="3"/>
-        <v>56971.529208072345</v>
+        <v>73042.24796375788</v>
       </c>
       <c r="E31">
         <f t="shared" si="4"/>
-        <v>623537.86885666777</v>
+        <v>321412.00006381638</v>
       </c>
       <c r="F31">
         <f t="shared" si="1"/>
-        <v>2516858.3298226255</v>
+        <v>1239153.693536975</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -3121,23 +3343,23 @@
       </c>
       <c r="B32">
         <f t="shared" si="2"/>
-        <v>93584.871015391938</v>
+        <v>45762.031238240525</v>
       </c>
       <c r="C32">
         <f t="shared" si="0"/>
-        <v>8550.6806864246319</v>
+        <v>10399.616792046136</v>
       </c>
       <c r="D32">
         <f t="shared" si="3"/>
-        <v>65522.209894496977</v>
+        <v>83441.86475580401</v>
       </c>
       <c r="E32">
         <f t="shared" si="4"/>
-        <v>717122.73987205967</v>
+        <v>367174.03130205692</v>
       </c>
       <c r="F32">
         <f t="shared" si="1"/>
-        <v>2901131.0014771502</v>
+        <v>1418622.9683854564</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -3146,23 +3368,23 @@
       </c>
       <c r="B33">
         <f t="shared" si="2"/>
-        <v>104031.91534178783</v>
+        <v>50535.164326967439</v>
       </c>
       <c r="C33">
         <f t="shared" si="0"/>
-        <v>9505.2082631869416</v>
+        <v>11484.331645759086</v>
       </c>
       <c r="D33">
         <f t="shared" si="3"/>
-        <v>75027.418157683918</v>
+        <v>94926.196401563095</v>
       </c>
       <c r="E33">
         <f t="shared" si="4"/>
-        <v>821154.65521384752</v>
+        <v>417709.19562902435</v>
       </c>
       <c r="F33">
         <f t="shared" si="1"/>
-        <v>3329021.2909372104</v>
+        <v>1617125.258462958</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -3171,23 +3393,23 @@
       </c>
       <c r="B34">
         <f t="shared" si="2"/>
-        <v>115269.16121705991</v>
+        <v>55636.020966749413</v>
       </c>
       <c r="C34">
         <f t="shared" si="0"/>
-        <v>10531.935128670259</v>
+        <v>12643.523074319812</v>
       </c>
       <c r="D34">
         <f t="shared" si="3"/>
-        <v>85559.353286354177</v>
+        <v>107569.71947588291</v>
       </c>
       <c r="E34">
         <f t="shared" si="4"/>
-        <v>936423.81643090746</v>
+        <v>473345.21659577376</v>
       </c>
       <c r="F34">
         <f t="shared" si="1"/>
-        <v>3803882.3201629771</v>
+        <v>1835988.6919027306</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -3196,23 +3418,23 @@
       </c>
       <c r="B35">
         <f t="shared" si="2"/>
-        <v>127329.70223741005</v>
+        <v>61076.144757749171</v>
       </c>
       <c r="C35">
         <f t="shared" si="0"/>
-        <v>11633.884985005252</v>
+        <v>13879.814410103314</v>
       </c>
       <c r="D35">
         <f t="shared" si="3"/>
-        <v>97193.238271359427</v>
+        <v>121449.53388598622</v>
       </c>
       <c r="E35">
         <f t="shared" si="4"/>
-        <v>1063753.5186683175</v>
+        <v>534421.36135352298</v>
       </c>
       <c r="F35">
         <f t="shared" si="1"/>
-        <v>4329209.876071942</v>
+        <v>2076588.9217634718</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -3221,23 +3443,23 @@
       </c>
       <c r="B36">
         <f t="shared" si="2"/>
-        <v>140246.9680493355</v>
+        <v>66867.123120990902</v>
       </c>
       <c r="C36">
         <f t="shared" si="0"/>
-        <v>12814.1122386313</v>
+        <v>15195.838943962273</v>
       </c>
       <c r="D36">
         <f t="shared" si="3"/>
-        <v>110007.35050999073</v>
+        <v>136645.37282994849</v>
       </c>
       <c r="E36">
         <f t="shared" si="4"/>
-        <v>1204000.486717653</v>
+        <v>601288.48447451391</v>
       </c>
       <c r="F36">
         <f t="shared" si="1"/>
-        <v>4908643.8817267427</v>
+        <v>2340349.3092346815</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -3246,23 +3468,23 @@
       </c>
       <c r="B37">
         <f t="shared" si="2"/>
-        <v>154054.71772442746</v>
+        <v>73020.586167899324</v>
       </c>
       <c r="C37">
         <f t="shared" si="0"/>
-        <v>14075.701394963808</v>
+        <v>16594.239668324975</v>
       </c>
       <c r="D37">
         <f t="shared" si="3"/>
-        <v>124083.05190495454</v>
+        <v>153239.61249827346</v>
       </c>
       <c r="E37">
         <f t="shared" si="4"/>
-        <v>1358055.2044420806</v>
+        <v>674309.07064241322</v>
       </c>
       <c r="F37">
         <f t="shared" si="1"/>
-        <v>5545969.8380793892</v>
+        <v>2628741.1020443756</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -3271,23 +3493,23 @@
       </c>
       <c r="B38">
         <f t="shared" si="2"/>
-        <v>168787.03345142218</v>
+        <v>79548.205630558019</v>
       </c>
       <c r="C38">
         <f t="shared" si="0"/>
-        <v>15421.76648204829</v>
+        <v>18077.66903409197</v>
       </c>
       <c r="D38">
         <f t="shared" si="3"/>
-        <v>139504.81838700283</v>
+        <v>171317.28153236542</v>
       </c>
       <c r="E38">
         <f t="shared" si="4"/>
-        <v>1526842.2378935027</v>
+        <v>753857.27627297118</v>
       </c>
       <c r="F38">
         <f t="shared" si="1"/>
-        <v>6245120.2377026202</v>
+        <v>2943283.6083306465</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -3296,23 +3518,23 @@
       </c>
       <c r="B39">
         <f t="shared" si="2"/>
-        <v>184478.31452187253</v>
+        <v>86461.693847823408</v>
       </c>
       <c r="C39">
         <f t="shared" si="0"/>
-        <v>16855.450501042054</v>
+        <v>19648.788720226137</v>
       </c>
       <c r="D39">
         <f t="shared" si="3"/>
-        <v>156360.26888804487</v>
+        <v>190966.07025259157</v>
       </c>
       <c r="E39">
         <f t="shared" si="4"/>
-        <v>1711320.5524153751</v>
+        <v>840318.97012079461</v>
       </c>
       <c r="F39">
         <f t="shared" si="1"/>
-        <v>7010175.9518311564</v>
+        <v>3285544.3662172896</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -3321,23 +3543,23 @@
       </c>
       <c r="B40">
         <f t="shared" si="2"/>
-        <v>201163.27158815716</v>
+        <v>93772.802802945458</v>
       </c>
       <c r="C40">
         <f t="shared" si="0"/>
-        <v>18379.924901578863</v>
+        <v>21310.269415047882</v>
       </c>
       <c r="D40">
         <f t="shared" si="3"/>
-        <v>174740.19378962374</v>
+        <v>212276.33966763946</v>
       </c>
       <c r="E40">
         <f t="shared" si="4"/>
-        <v>1912483.8240035323</v>
+        <v>934091.77292374009</v>
       </c>
       <c r="F40">
         <f t="shared" si="1"/>
-        <v>7845367.5919381296</v>
+        <v>3657139.3093148731</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -3346,23 +3568,23 @@
       </c>
       <c r="B41">
         <f t="shared" si="2"/>
-        <v>218876.92117461699</v>
+        <v>101493.32320878371</v>
       </c>
       <c r="C41">
         <f t="shared" si="0"/>
-        <v>19998.389080261382</v>
+        <v>23064.790608346582</v>
       </c>
       <c r="D41">
         <f t="shared" si="3"/>
-        <v>194738.58286988511</v>
+        <v>235341.13027598604</v>
       </c>
       <c r="E41">
         <f t="shared" si="4"/>
-        <v>2131360.7451781491</v>
+        <v>1035585.0961325238</v>
       </c>
       <c r="F41">
         <f t="shared" si="1"/>
-        <v>8755076.8469846789</v>
+        <v>4059732.9283513483</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -3371,23 +3593,23 @@
       </c>
       <c r="B42">
         <f t="shared" si="2"/>
-        <v>237654.58042441815</v>
+        <v>109635.08363710482</v>
       </c>
       <c r="C42">
         <f t="shared" si="0"/>
-        <v>21714.069900691531</v>
+        <v>24915.040393509753</v>
       </c>
       <c r="D42">
         <f t="shared" si="3"/>
-        <v>216452.65277057665</v>
+        <v>260256.1706694958</v>
       </c>
       <c r="E42">
         <f t="shared" si="4"/>
-        <v>2369015.3256025673</v>
+        <v>1145220.1797696287</v>
       </c>
       <c r="F42">
         <f t="shared" si="1"/>
-        <v>9743837.7974011432</v>
+        <v>4495038.4291212978</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -3396,23 +3618,23 @@
       </c>
       <c r="B43">
         <f t="shared" si="2"/>
-        <v>257531.8620663473</v>
+        <v>118209.94968878325</v>
       </c>
       <c r="C43">
         <f t="shared" si="0"/>
-        <v>23530.221233595679</v>
+        <v>26863.715278947599</v>
       </c>
       <c r="D43">
         <f t="shared" si="3"/>
-        <v>239982.87400417234</v>
+        <v>287119.88594844338</v>
       </c>
       <c r="E43">
         <f t="shared" si="4"/>
-        <v>2626547.1876689144</v>
+        <v>1263430.1294584118</v>
       </c>
       <c r="F43">
         <f t="shared" si="1"/>
-        <v>10816338.206786586</v>
+        <v>4964817.8869288964</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -3421,23 +3643,23 @@
       </c>
       <c r="B44">
         <f t="shared" si="2"/>
-        <v>278544.66958716715</v>
+        <v>127229.82320203212</v>
       </c>
       <c r="C44">
         <f t="shared" si="0"/>
-        <v>25450.123515731448</v>
+        <v>28913.520008160089</v>
       </c>
       <c r="D44">
         <f t="shared" si="3"/>
-        <v>265432.99751990376</v>
+        <v>316033.40595660347</v>
       </c>
       <c r="E44">
         <f t="shared" si="4"/>
-        <v>2905091.8572560814</v>
+        <v>1390659.952660444</v>
       </c>
       <c r="F44">
         <f t="shared" si="1"/>
-        <v>11977420.792248188</v>
+        <v>5470882.3976873811</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -3446,23 +3668,23 @@
       </c>
       <c r="B45">
         <f t="shared" si="2"/>
-        <v>300729.19259641477</v>
+        <v>136706.64149605282</v>
       </c>
       <c r="C45">
         <f t="shared" si="0"/>
-        <v>27477.083326377739</v>
+        <v>31067.167387853126</v>
       </c>
       <c r="D45">
         <f t="shared" si="3"/>
-        <v>292910.08084628149</v>
+        <v>347100.57334445661</v>
       </c>
       <c r="E45">
         <f t="shared" si="4"/>
-        <v>3205821.049852496</v>
+        <v>1527366.5941564967</v>
       </c>
       <c r="F45">
         <f t="shared" si="1"/>
-        <v>13232084.47424225</v>
+        <v>6015092.225826324</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -3471,23 +3693,23 @@
       </c>
       <c r="B46">
         <f t="shared" si="2"/>
-        <v>324121.90237165644</v>
+        <v>146652.37664773178</v>
       </c>
       <c r="C46">
         <f t="shared" si="0"/>
-        <v>29614.432980312697</v>
+        <v>33327.378123564798</v>
       </c>
       <c r="D46">
         <f t="shared" si="3"/>
-        <v>322524.51382659416</v>
+        <v>380427.95146802143</v>
       </c>
       <c r="E46">
         <f t="shared" si="4"/>
-        <v>3529942.9522241526</v>
+        <v>1674018.9708042284</v>
       </c>
       <c r="F46">
         <f t="shared" si="1"/>
-        <v>14585485.60672454</v>
+        <v>6599356.9491479304</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -3496,23 +3718,23 @@
       </c>
       <c r="B47">
         <f t="shared" si="2"/>
-        <v>348759.54757320805</v>
+        <v>157079.03479921928</v>
       </c>
       <c r="C47">
         <f t="shared" si="0"/>
-        <v>31865.530136275451</v>
+        <v>35696.880662309697</v>
       </c>
       <c r="D47">
         <f t="shared" si="3"/>
-        <v>354390.04396286962</v>
+        <v>416124.83213033114</v>
       </c>
       <c r="E47">
         <f t="shared" si="4"/>
-        <v>3878702.4997973605</v>
+        <v>1831098.0056034478</v>
       </c>
       <c r="F47">
         <f t="shared" si="1"/>
-        <v>16042939.18836757</v>
+        <v>7225635.6007640874</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -3521,23 +3743,23 @@
       </c>
       <c r="B48">
         <f t="shared" si="2"/>
-        <v>374679.15011823928</v>
+        <v>167998.65549441447</v>
       </c>
       <c r="C48">
         <f t="shared" si="0"/>
-        <v>34233.757419990463</v>
+        <v>38178.411041792315</v>
       </c>
       <c r="D48">
         <f t="shared" si="3"/>
-        <v>388623.80138286005</v>
+        <v>454303.24317212345</v>
       </c>
       <c r="E48">
         <f t="shared" si="4"/>
-        <v>4253381.6499156002</v>
+        <v>1999096.6610978623</v>
       </c>
       <c r="F48">
         <f t="shared" si="1"/>
-        <v>17609920.055557247</v>
+        <v>7895936.80823748</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -3546,23 +3768,23 @@
       </c>
       <c r="B49">
         <f t="shared" si="2"/>
-        <v>401918.00120498368</v>
+        <v>179423.31104254554</v>
       </c>
       <c r="C49">
         <f t="shared" si="0"/>
-        <v>36722.522060906776</v>
+        <v>40774.712745777928</v>
       </c>
       <c r="D49">
         <f t="shared" si="3"/>
-        <v>425346.3234437668</v>
+        <v>495077.95591790136</v>
       </c>
       <c r="E49">
         <f t="shared" si="4"/>
-        <v>4655299.6511205835</v>
+        <v>2178519.9721404077</v>
       </c>
       <c r="F49">
         <f t="shared" si="1"/>
-        <v>19292064.057839215</v>
+        <v>8612318.9300421849</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -3571,23 +3793,23 @@
       </c>
       <c r="B50">
         <f t="shared" si="2"/>
-        <v>430513.65747849172</v>
+        <v>191365.10590718305</v>
       </c>
       <c r="C50">
         <f t="shared" si="0"/>
-        <v>39335.255541869818</v>
+        <v>43488.536565243274</v>
       </c>
       <c r="D50">
         <f t="shared" si="3"/>
-        <v>464681.57898563659</v>
+        <v>538566.49248314463</v>
       </c>
       <c r="E50">
         <f t="shared" si="4"/>
-        <v>5085813.3085990753</v>
+        <v>2369885.0780475908</v>
       </c>
       <c r="F50">
         <f t="shared" si="1"/>
-        <v>21095169.216446094</v>
+        <v>9376890.1894519702</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -3596,23 +3818,23 @@
       </c>
       <c r="B51">
         <f t="shared" si="2"/>
-        <v>460503.93733004777</v>
+        <v>203836.1761191641</v>
       </c>
       <c r="C51">
         <f t="shared" si="0"/>
-        <v>42075.413261005793</v>
+        <v>46322.640464961063</v>
       </c>
       <c r="D51">
         <f t="shared" si="3"/>
-        <v>506756.99224664236</v>
+        <v>584889.13294810569</v>
       </c>
       <c r="E51">
         <f t="shared" si="4"/>
-        <v>5546317.2459291229</v>
+        <v>2573721.2541667549</v>
       </c>
       <c r="F51">
         <f t="shared" si="1"/>
-        <v>23025196.866502389</v>
+        <v>10191808.805958204</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -3621,23 +3843,23 @@
       </c>
       <c r="B52">
         <f t="shared" si="2"/>
-        <v>491926.91732292878</v>
+        <v>216848.68871201618</v>
       </c>
       <c r="C52">
         <f t="shared" si="0"/>
-        <v>44946.474205149687</v>
+        <v>49279.789455197613</v>
       </c>
       <c r="D52">
         <f t="shared" si="3"/>
-        <v>551703.46645179205</v>
+        <v>634168.92240330332</v>
       </c>
       <c r="E52">
         <f t="shared" si="4"/>
-        <v>6038244.1632520519</v>
+        <v>2790569.9428787711</v>
       </c>
       <c r="F52">
         <f t="shared" si="1"/>
-        <v>25088272.783469368</v>
+        <v>11059283.124312826</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -3646,23 +3868,23 @@
       </c>
       <c r="B53">
         <f t="shared" si="2"/>
-        <v>524820.92873775947</v>
+        <v>230414.84117859136</v>
       </c>
       <c r="C53">
         <f t="shared" si="0"/>
-        <v>47951.940634200633</v>
+        <v>52362.755468230687</v>
       </c>
       <c r="D53">
         <f t="shared" si="3"/>
-        <v>599655.40708599263</v>
+        <v>686531.67787153402</v>
       </c>
       <c r="E53">
         <f t="shared" si="4"/>
-        <v>6563065.0919898115</v>
+        <v>3020984.7840573625</v>
       </c>
       <c r="F53">
         <f t="shared" si="1"/>
-        <v>27290688.294363491</v>
+        <v>11981571.741286751</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -3671,23 +3893,23 @@
       </c>
       <c r="B54">
         <f t="shared" si="2"/>
-        <v>559224.55423117056</v>
+        <v>244546.86094770508</v>
       </c>
       <c r="C54">
         <f t="shared" si="0"/>
-        <v>51095.337775829576</v>
+        <v>55574.317239413409</v>
       </c>
       <c r="D54">
         <f t="shared" si="3"/>
-        <v>650750.74486182223</v>
+        <v>742105.99511094741</v>
       </c>
       <c r="E54">
         <f t="shared" si="4"/>
-        <v>7122289.6462209821</v>
+        <v>3265531.6450050673</v>
       </c>
       <c r="F54">
         <f t="shared" si="1"/>
-        <v>29638901.37425204</v>
+        <v>12960983.630228369</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -3696,23 +3918,23 @@
       </c>
       <c r="B55">
         <f t="shared" si="2"/>
-        <v>595176.62460193818</v>
+        <v>259257.00487967944</v>
       </c>
       <c r="C55">
         <f t="shared" si="0"/>
-        <v>54380.213530007211</v>
+        <v>58917.260192534348</v>
       </c>
       <c r="D55">
         <f t="shared" si="3"/>
-        <v>705130.95839182939</v>
+        <v>801023.25530348171</v>
       </c>
       <c r="E55">
         <f t="shared" si="4"/>
-        <v>7717466.2708229199</v>
+        <v>3524788.6498847469</v>
       </c>
       <c r="F55">
         <f t="shared" si="1"/>
-        <v>32139537.728504661</v>
+        <v>13999878.263502689</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -3721,23 +3943,23 @@
       </c>
       <c r="B56">
         <f t="shared" si="2"/>
-        <v>632716.21565917635</v>
+        <v>274557.55877976085</v>
       </c>
       <c r="C56">
         <f t="shared" si="0"/>
-        <v>57810.138182856404</v>
+        <v>62394.376329239545</v>
       </c>
       <c r="D56">
         <f t="shared" si="3"/>
-        <v>762941.09657468577</v>
+        <v>863417.63163272128</v>
       </c>
       <c r="E56">
         <f t="shared" si="4"/>
-        <v>8350182.4864820959</v>
+        <v>3799346.2086645076</v>
       </c>
       <c r="F56">
         <f t="shared" si="1"/>
-        <v>34799391.8612547</v>
+        <v>15100665.732886847</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -3746,23 +3968,23 @@
       </c>
       <c r="B57">
         <f t="shared" si="2"/>
-        <v>671882.64518751227</v>
+        <v>290460.83692845242</v>
       </c>
       <c r="C57">
         <f t="shared" si="0"/>
-        <v>61388.704129365775</v>
+        <v>66008.464122298625</v>
       </c>
       <c r="D57">
         <f t="shared" si="3"/>
-        <v>824329.80070405151</v>
+        <v>929426.09575501992</v>
       </c>
       <c r="E57">
         <f t="shared" si="4"/>
-        <v>9022065.1316696089</v>
+        <v>4089807.04559296</v>
       </c>
       <c r="F57">
         <f t="shared" si="1"/>
-        <v>37625428.130500689</v>
+        <v>16265806.867993336</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -3771,23 +3993,23 @@
       </c>
       <c r="B58">
         <f t="shared" si="2"/>
-        <v>712715.47000454483</v>
+        <v>306979.18162788922</v>
       </c>
       <c r="C58">
         <f t="shared" si="0"/>
-        <v>65119.525604534938</v>
+        <v>69762.328412516566</v>
       </c>
       <c r="D58">
         <f t="shared" si="3"/>
-        <v>889449.3263085864</v>
+        <v>999188.42416753643</v>
       </c>
       <c r="E58">
         <f t="shared" si="4"/>
-        <v>9734780.6016741544</v>
+        <v>4396786.2272208491</v>
       </c>
       <c r="F58">
         <f t="shared" si="1"/>
-        <v>40624781.790259056</v>
+        <v>17497813.352789685</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -3796,23 +4018,23 @@
       </c>
       <c r="B59">
         <f t="shared" si="2"/>
-        <v>755254.48310616915</v>
+        <v>324124.96276341862</v>
       </c>
       <c r="C59">
         <f t="shared" si="0"/>
-        <v>69006.23842254802</v>
+        <v>73658.780309101028</v>
       </c>
       <c r="D59">
         <f t="shared" si="3"/>
-        <v>958455.56473113445</v>
+        <v>1072847.2044766375</v>
       </c>
       <c r="E59">
         <f t="shared" si="4"/>
-        <v>10490035.084780324</v>
+        <v>4720911.1899842676</v>
       </c>
       <c r="F59">
         <f t="shared" si="1"/>
-        <v>43804760.020157814</v>
+        <v>18799247.840278279</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -3821,23 +4043,23 @@
       </c>
       <c r="B60">
         <f t="shared" si="2"/>
-        <v>799539.71089563461</v>
+        <v>341910.57737962552</v>
       </c>
       <c r="C60">
         <f t="shared" si="0"/>
-        <v>73052.499723597604</v>
+        <v>77700.637093312209</v>
       </c>
       <c r="D60">
         <f t="shared" si="3"/>
-        <v>1031508.064454732</v>
+        <v>1150547.8415699496</v>
       </c>
       <c r="E60">
         <f t="shared" si="4"/>
-        <v>11289574.795675959</v>
+        <v>5062821.7673638929</v>
       </c>
       <c r="F60">
         <f t="shared" si="1"/>
-        <v>47172842.942842439</v>
+        <v>20172724.065397907</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -3846,23 +4068,23 @@
       </c>
       <c r="B61">
         <f t="shared" si="2"/>
-        <v>845611.41049247223</v>
+        <v>360348.44927007589</v>
       </c>
       <c r="C61">
         <f t="shared" si="0"/>
-        <v>77261.987728006396</v>
+        <v>81890.722125230372</v>
       </c>
       <c r="D61">
         <f t="shared" si="3"/>
-        <v>1108770.0521827384</v>
+        <v>1232438.56369518</v>
       </c>
       <c r="E61">
         <f t="shared" si="4"/>
-        <v>12135186.206168432</v>
+        <v>5423170.216633969</v>
       </c>
       <c r="F61">
         <f t="shared" si="1"/>
-        <v>50736684.629548334</v>
+        <v>21620906.956204552</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -3871,23 +4093,23 @@
       </c>
       <c r="B62">
         <f t="shared" si="2"/>
-        <v>893510.06711771304</v>
+        <v>379451.02858012915</v>
       </c>
       <c r="C62">
         <f t="shared" si="0"/>
-        <v>81638.401497319282</v>
+        <v>86231.864753493239</v>
       </c>
       <c r="D62">
         <f t="shared" si="3"/>
-        <v>1190408.4536800578</v>
+        <v>1318670.4284486733</v>
       </c>
       <c r="E62">
         <f t="shared" si="4"/>
-        <v>13028696.273286145</v>
+        <v>5802621.2452140981</v>
       </c>
       <c r="F62">
         <f t="shared" si="1"/>
-        <v>54504114.094180495</v>
+        <v>23146512.743387878</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -3896,23 +4118,23 @@
       </c>
       <c r="B63">
         <f t="shared" si="2"/>
-        <v>943276.39155191032</v>
+        <v>399230.79142216319</v>
       </c>
       <c r="C63">
         <f t="shared" si="0"/>
-        <v>86185.460702047421</v>
+        <v>90726.900227854247</v>
       </c>
       <c r="D63">
         <f t="shared" si="3"/>
-        <v>1276593.9143821052</v>
+        <v>1409397.3286765276</v>
       </c>
       <c r="E63">
         <f t="shared" si="4"/>
-        <v>13971972.664838055</v>
+        <v>6201852.0366362613</v>
       </c>
       <c r="F63">
         <f t="shared" si="1"/>
-        <v>58483136.276218437</v>
+        <v>24752309.068174116</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -3921,23 +4143,23 @@
       </c>
       <c r="B64">
         <f t="shared" si="2"/>
-        <v>994951.31766286748</v>
+        <v>419700.23950265336</v>
       </c>
       <c r="C64">
         <f t="shared" si="0"/>
-        <v>90906.905395781185</v>
+        <v>95378.669614434621</v>
       </c>
       <c r="D64">
         <f t="shared" si="3"/>
-        <v>1367500.8197778864</v>
+        <v>1504775.9982909623</v>
       </c>
       <c r="E64">
         <f t="shared" si="4"/>
-        <v>14966923.982500922</v>
+        <v>6621552.2761389147</v>
       </c>
       <c r="F64">
         <f t="shared" si="1"/>
-        <v>62681933.012760654</v>
+        <v>26441115.088667162</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -3946,23 +4168,23 @@
       </c>
       <c r="B65">
         <f t="shared" si="2"/>
-        <v>1048575.9999999981</v>
+        <v>440871.89976053999</v>
       </c>
       <c r="C65">
         <f t="shared" si="0"/>
-        <v>95806.495795391238</v>
+        <v>100190.01971354091</v>
       </c>
       <c r="D65">
         <f t="shared" si="3"/>
-        <v>1463307.3155732777</v>
+        <v>1604966.0180045031</v>
       </c>
       <c r="E65">
         <f t="shared" si="4"/>
-        <v>16015499.98250092</v>
+        <v>7062424.1758994544</v>
       </c>
       <c r="F65">
         <f t="shared" si="1"/>
-        <v>67108863.999999881</v>
+        <v>28215801.58467456</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -3971,23 +4193,23 @@
       </c>
       <c r="B66">
         <f t="shared" si="2"/>
-        <v>1104191.8114525175</v>
+        <v>462758.32401636994</v>
       </c>
       <c r="C66">
         <f t="shared" si="0"/>
-        <v>100888.01206706166</v>
+        <v>105163.80297993086</v>
       </c>
       <c r="D66">
         <f t="shared" si="3"/>
-        <v>1564195.3276403393</v>
+        <v>1710129.8209844339</v>
       </c>
       <c r="E66">
         <f t="shared" si="4"/>
-        <v>17119691.793953437</v>
+        <v>7525182.4999158243</v>
       </c>
       <c r="F66">
         <f t="shared" si="1"/>
-        <v>71772467.744413644</v>
+        <v>30079291.061064046</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -3996,23 +4218,23 @@
       </c>
       <c r="B67">
         <f t="shared" si="2"/>
-        <v>1161840.3409687951</v>
+        <v>485372.08863173251</v>
       </c>
       <c r="C67">
-        <f t="shared" ref="C67:C101" si="5">B67/SUM($B$2:$B$101)*$I$5</f>
-        <v>106155.25411791133</v>
+        <f t="shared" ref="C67:C101" si="5">B67/SUM(B:B)*$I$5</f>
+        <v>110302.8774454188</v>
       </c>
       <c r="D67">
         <f t="shared" si="3"/>
-        <v>1670350.5817582505</v>
+        <v>1820432.6984298527</v>
       </c>
       <c r="E67">
         <f t="shared" si="4"/>
-        <v>18281532.134922232</v>
+        <v>8010554.5885475567</v>
       </c>
       <c r="F67">
         <f t="shared" ref="F67:F101" si="6">A67*B67</f>
-        <v>76681462.503940478</v>
+        <v>32034557.849694345</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -4021,23 +4243,23 @@
       </c>
       <c r="B68">
         <f t="shared" ref="B68:B101" si="7">A68^(1/(1-$I$1))</f>
-        <v>1221563.3913343418</v>
+        <v>508725.79417853244</v>
       </c>
       <c r="C68">
         <f t="shared" si="5"/>
-        <v>111612.04139297266</v>
+        <v>115610.1066437165</v>
       </c>
       <c r="D68">
         <f t="shared" ref="D68:D101" si="8">D67+C68</f>
-        <v>1781962.6231512232</v>
+        <v>1936042.8050735693</v>
       </c>
       <c r="E68">
         <f t="shared" ref="E68:E101" si="9">E67+B68</f>
-        <v>19503095.526256576</v>
+        <v>8519280.3827260882</v>
       </c>
       <c r="F68">
         <f t="shared" si="6"/>
-        <v>81844747.219400898</v>
+        <v>34084628.209961675</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -4046,23 +4268,23 @@
       </c>
       <c r="B69">
         <f t="shared" si="7"/>
-        <v>1283402.9770060752</v>
+        <v>532832.06511766522</v>
       </c>
       <c r="C69">
         <f t="shared" si="5"/>
-        <v>117262.21267731224</v>
+        <v>121088.35953741077</v>
       </c>
       <c r="D69">
         <f t="shared" si="8"/>
-        <v>1899224.8358285355</v>
+        <v>2057131.1646109801</v>
       </c>
       <c r="E69">
         <f t="shared" si="9"/>
-        <v>20786498.50326265</v>
+        <v>9052112.4478437528</v>
       </c>
       <c r="F69">
         <f t="shared" si="6"/>
-        <v>87271402.436413109</v>
+        <v>36232580.428001232</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -4071,23 +4293,23 @@
       </c>
       <c r="B70">
         <f t="shared" si="7"/>
-        <v>1347401.3220005883</v>
+        <v>557703.54948669509</v>
       </c>
       <c r="C70">
         <f t="shared" si="5"/>
-        <v>123109.62590308588</v>
+        <v>126740.51044698698</v>
       </c>
       <c r="D70">
         <f t="shared" si="8"/>
-        <v>2022334.4617316213</v>
+        <v>2183871.6750579672</v>
       </c>
       <c r="E70">
         <f t="shared" si="9"/>
-        <v>22133899.825263239</v>
+        <v>9609815.9973304477</v>
       </c>
       <c r="F70">
         <f t="shared" si="6"/>
-        <v>92970691.218040586</v>
+        <v>38481544.914581962</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -4096,23 +4318,23 @@
       </c>
       <c r="B71">
         <f t="shared" si="7"/>
-        <v>1413600.8578343359</v>
+        <v>583352.91859616467</v>
       </c>
       <c r="C71">
         <f t="shared" si="5"/>
-        <v>129158.15796133708</v>
+        <v>132569.43898181408</v>
       </c>
       <c r="D71">
         <f t="shared" si="8"/>
-        <v>2151492.6196929584</v>
+        <v>2316441.1140397815</v>
       </c>
       <c r="E71">
         <f t="shared" si="9"/>
-        <v>23547500.683097575</v>
+        <v>10193168.915926613</v>
       </c>
       <c r="F71">
         <f t="shared" si="6"/>
-        <v>98952060.048403516</v>
+        <v>40834704.301731527</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -4121,23 +4343,23 @@
       </c>
       <c r="B72">
         <f t="shared" si="7"/>
-        <v>1482044.2215136804</v>
+        <v>609792.86673414905</v>
       </c>
       <c r="C72">
         <f t="shared" si="5"/>
-        <v>135411.70451835112</v>
+        <v>138578.02997300329</v>
       </c>
       <c r="D72">
         <f t="shared" si="8"/>
-        <v>2286904.3242113097</v>
+        <v>2455019.1440127846</v>
       </c>
       <c r="E72">
         <f t="shared" si="9"/>
-        <v>25029544.904611256</v>
+        <v>10802961.782660762</v>
       </c>
       <c r="F72">
         <f t="shared" si="6"/>
-        <v>105225139.72747131</v>
+        <v>43295293.538124584</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -4146,23 +4368,23 @@
       </c>
       <c r="B73">
         <f t="shared" si="7"/>
-        <v>1552774.2535729534</v>
+        <v>637036.11087875324</v>
       </c>
       <c r="C73">
         <f t="shared" si="5"/>
-        <v>141874.17983639639</v>
+        <v>144769.17340807192</v>
       </c>
       <c r="D73">
         <f t="shared" si="8"/>
-        <v>2428778.5040477063</v>
+        <v>2599788.3174208566</v>
       </c>
       <c r="E73">
         <f t="shared" si="9"/>
-        <v>26582319.158184208</v>
+        <v>11439997.893539514</v>
       </c>
       <c r="F73">
         <f t="shared" si="6"/>
-        <v>111799746.25725265</v>
+        <v>45866599.983270235</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -4171,23 +4393,23 @@
       </c>
       <c r="B74">
         <f t="shared" si="7"/>
-        <v>1625833.9961586357</v>
+        <v>665095.39041818527</v>
       </c>
       <c r="C74">
         <f t="shared" si="5"/>
-        <v>148549.5165986793</v>
+        <v>151145.76436732875</v>
       </c>
       <c r="D74">
         <f t="shared" si="8"/>
-        <v>2577328.0206463854</v>
+        <v>2750934.0817881855</v>
       </c>
       <c r="E74">
         <f t="shared" si="9"/>
-        <v>28208153.154342845</v>
+        <v>12105093.283957699</v>
       </c>
       <c r="F74">
         <f t="shared" si="6"/>
-        <v>118685881.71958041</v>
+        <v>48551963.500527523</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -4196,23 +4418,23 @@
       </c>
       <c r="B75">
         <f t="shared" si="7"/>
-        <v>1701266.6911580598</v>
+        <v>693983.46687815641</v>
       </c>
       <c r="C75">
         <f t="shared" si="5"/>
-        <v>155441.66573836718</v>
+        <v>157710.70296192469</v>
       </c>
       <c r="D75">
         <f t="shared" si="8"/>
-        <v>2732769.6863847524</v>
+        <v>2908644.78475011</v>
       </c>
       <c r="E75">
         <f t="shared" si="9"/>
-        <v>29909419.845500905</v>
+        <v>12799076.750835856</v>
       </c>
       <c r="F75">
         <f t="shared" si="6"/>
-        <v>125893735.14569642</v>
+        <v>51354776.548983574</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -4221,23 +4443,23 @@
       </c>
       <c r="B76">
         <f t="shared" si="7"/>
-        <v>1779115.7783708724</v>
+        <v>723713.12365625612</v>
       </c>
       <c r="C76">
         <f t="shared" si="5"/>
-        <v>162554.59627151824</v>
+        <v>164466.89427348808</v>
       </c>
       <c r="D76">
         <f t="shared" si="8"/>
-        <v>2895324.2826562705</v>
+        <v>3073111.6790235983</v>
       </c>
       <c r="E76">
         <f t="shared" si="9"/>
-        <v>31688535.623871777</v>
+        <v>13522789.874492113</v>
       </c>
       <c r="F76">
         <f t="shared" si="6"/>
-        <v>133433683.37781543</v>
+        <v>54278484.274219207</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -4246,23 +4468,23 @@
       </c>
       <c r="B77">
         <f t="shared" si="7"/>
-        <v>1859424.8937218725</v>
+        <v>754297.16576310084</v>
       </c>
       <c r="C77">
         <f t="shared" si="5"/>
-        <v>169892.29513379163</v>
+        <v>171417.2482953</v>
       </c>
       <c r="D77">
         <f t="shared" si="8"/>
-        <v>3065216.5777900619</v>
+        <v>3244528.9273188985</v>
       </c>
       <c r="E77">
         <f t="shared" si="9"/>
-        <v>33547960.517593648</v>
+        <v>14277087.040255213</v>
       </c>
       <c r="F77">
         <f t="shared" si="6"/>
-        <v>141316291.92286232</v>
+        <v>57326584.597995661</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -4271,23 +4493,23 @@
       </c>
       <c r="B78">
         <f t="shared" si="7"/>
-        <v>1942237.8675135483</v>
+        <v>785748.41956993076</v>
       </c>
       <c r="C78">
         <f t="shared" si="5"/>
-        <v>177458.76702078508</v>
+        <v>178564.67987493434</v>
       </c>
       <c r="D78">
         <f t="shared" si="8"/>
-        <v>3242675.3448108472</v>
+        <v>3423093.6071938328</v>
       </c>
       <c r="E78">
         <f t="shared" si="9"/>
-        <v>35490198.385107197</v>
+        <v>15062835.459825143</v>
       </c>
       <c r="F78">
         <f t="shared" si="6"/>
-        <v>149552315.79854321</v>
+        <v>60502628.306884669</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -4296,23 +4518,23 @@
       </c>
       <c r="B79">
         <f t="shared" si="7"/>
-        <v>2027598.7227171059</v>
+        <v>818079.73256245139</v>
       </c>
       <c r="C79">
         <f t="shared" si="5"/>
-        <v>185258.03423188915</v>
+        <v>185912.1086583173</v>
       </c>
       <c r="D79">
         <f t="shared" si="8"/>
-        <v>3427933.3790427363</v>
+        <v>3609005.7158521502</v>
       </c>
       <c r="E79">
         <f t="shared" si="9"/>
-        <v>37517797.107824303</v>
+        <v>15880915.192387594</v>
       </c>
       <c r="F79">
         <f t="shared" si="6"/>
-        <v>158152700.37193426</v>
+        <v>63810219.13987121</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -4321,23 +4543,23 @@
       </c>
       <c r="B80">
         <f t="shared" si="7"/>
-        <v>2115551.6733005717</v>
+        <v>851303.97310068656</v>
       </c>
       <c r="C80">
         <f t="shared" si="5"/>
-        <v>193294.136517529</v>
+        <v>193462.45903515286</v>
       </c>
       <c r="D80">
         <f t="shared" si="8"/>
-        <v>3621227.5155602652</v>
+        <v>3802468.1748873033</v>
       </c>
       <c r="E80">
         <f t="shared" si="9"/>
-        <v>39633348.781124875</v>
+        <v>16732219.16548828</v>
       </c>
       <c r="F80">
         <f t="shared" si="6"/>
-        <v>167128582.19074517</v>
+        <v>67253013.874954239</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -4346,23 +4568,23 @@
       </c>
       <c r="B81">
         <f t="shared" si="7"/>
-        <v>2206141.1225926448</v>
+        <v>885434.03018458211</v>
       </c>
       <c r="C81">
         <f t="shared" si="5"/>
-        <v>201571.13092967254</v>
+        <v>201218.66008565546</v>
       </c>
       <c r="D81">
         <f t="shared" si="8"/>
-        <v>3822798.6464899378</v>
+        <v>4003686.8349729585</v>
       </c>
       <c r="E81">
         <f t="shared" si="9"/>
-        <v>41839489.903717518</v>
+        <v>17617653.195672862</v>
       </c>
       <c r="F81">
         <f t="shared" si="6"/>
-        <v>176491289.80741158</v>
+        <v>70834722.414766565</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -4371,23 +4593,23 @@
       </c>
       <c r="B82">
         <f t="shared" si="7"/>
-        <v>2299411.6616812195</v>
+        <v>920482.81322521414</v>
       </c>
       <c r="C82">
         <f t="shared" si="5"/>
-        <v>210093.09167550632</v>
+        <v>209183.64552855582</v>
       </c>
       <c r="D82">
         <f t="shared" si="8"/>
-        <v>4032891.7381654442</v>
+        <v>4212870.4805015139</v>
       </c>
       <c r="E82">
         <f t="shared" si="9"/>
-        <v>44138901.565398738</v>
+        <v>18538136.008898076</v>
       </c>
       <c r="F82">
         <f t="shared" si="6"/>
-        <v>186252344.59617877</v>
+        <v>74559107.871242344</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -4396,23 +4618,23 @@
       </c>
       <c r="B83">
         <f t="shared" si="7"/>
-        <v>2395408.0678452658</v>
+        <v>956463.25182132097</v>
       </c>
       <c r="C83">
         <f t="shared" si="5"/>
-        <v>218864.10997415936</v>
+        <v>217360.35367031716</v>
       </c>
       <c r="D83">
         <f t="shared" si="8"/>
-        <v>4251755.8481396036</v>
+        <v>4430230.8341718307</v>
       </c>
       <c r="E83">
         <f t="shared" si="9"/>
-        <v>46534309.633244</v>
+        <v>19494599.260719396</v>
       </c>
       <c r="F83">
         <f t="shared" si="6"/>
-        <v>196423461.56331179</v>
+        <v>78429986.649348319</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -4421,23 +4643,23 @@
       </c>
       <c r="B84">
         <f t="shared" si="7"/>
-        <v>2494175.3030191455</v>
+        <v>993388.29554105748</v>
       </c>
       <c r="C84">
         <f t="shared" si="5"/>
-        <v>227888.29391639028</v>
+        <v>225751.72735553765</v>
       </c>
       <c r="D84">
         <f t="shared" si="8"/>
-        <v>4479644.1420559939</v>
+        <v>4655982.5615273686</v>
       </c>
       <c r="E84">
         <f t="shared" si="9"/>
-        <v>49028484.936263144</v>
+        <v>20487987.556260455</v>
       </c>
       <c r="F84">
         <f t="shared" si="6"/>
-        <v>207016550.15058908</v>
+        <v>82451228.529907778</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -4446,23 +4668,23 @@
       </c>
       <c r="B85">
         <f t="shared" si="7"/>
-        <v>2595758.5122881047</v>
+        <v>1031270.9137087123</v>
       </c>
       <c r="C85">
         <f t="shared" si="5"/>
-        <v>237169.7683271234</v>
+        <v>234360.7139184812</v>
       </c>
       <c r="D85">
         <f t="shared" si="8"/>
-        <v>4716813.9103831174</v>
+        <v>4890343.2754458496</v>
       </c>
       <c r="E85">
         <f t="shared" si="9"/>
-        <v>51624243.448551252</v>
+        <v>21519258.469969168</v>
       </c>
       <c r="F85">
         <f t="shared" si="6"/>
-        <v>218043715.03220081</v>
+        <v>86626756.751531839</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -4471,23 +4693,23 @@
       </c>
       <c r="B86">
         <f t="shared" si="7"/>
-        <v>2700203.0224141404</v>
+        <v>1070124.0951962706</v>
       </c>
       <c r="C86">
         <f t="shared" si="5"/>
-        <v>246712.67463075975</v>
+        <v>243190.26513570908</v>
       </c>
       <c r="D86">
         <f t="shared" si="8"/>
-        <v>4963526.5850138776</v>
+        <v>5133533.5405815588</v>
       </c>
       <c r="E86">
         <f t="shared" si="9"/>
-        <v>54324446.470965393</v>
+        <v>22589382.565165438</v>
       </c>
       <c r="F86">
         <f t="shared" si="6"/>
-        <v>229517256.90520194</v>
+        <v>90960548.091683</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -4496,23 +4718,23 @@
       </c>
       <c r="B87">
         <f t="shared" si="7"/>
-        <v>2807554.3403910659</v>
+        <v>1109960.8482195956</v>
       </c>
       <c r="C87">
         <f t="shared" si="5"/>
-        <v>256521.17071915584</v>
+        <v>252243.33717976141</v>
       </c>
       <c r="D87">
         <f t="shared" si="8"/>
-        <v>5220047.7557330336</v>
+        <v>5385776.8777613202</v>
       </c>
       <c r="E87">
         <f t="shared" si="9"/>
-        <v>57132000.811356455</v>
+        <v>23699343.413385034</v>
       </c>
       <c r="F87">
         <f t="shared" si="6"/>
-        <v>241449673.27363166</v>
+        <v>95456632.946885228</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -4521,23 +4743,23 @@
       </c>
       <c r="B88">
         <f t="shared" si="7"/>
-        <v>2917858.1520281178</v>
+        <v>1150794.2001391768</v>
       </c>
       <c r="C88">
         <f t="shared" si="5"/>
-        <v>266599.43082221068</v>
+        <v>261522.89057387633</v>
       </c>
       <c r="D88">
         <f t="shared" si="8"/>
-        <v>5486647.186555244</v>
+        <v>5647299.7683351962</v>
       </c>
       <c r="E88">
         <f t="shared" si="9"/>
-        <v>60049858.963384576</v>
+        <v>24850137.61352421</v>
       </c>
       <c r="F88">
         <f t="shared" si="6"/>
-        <v>253853659.22644624</v>
+        <v>100119095.41210838</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -4546,23 +4768,23 @@
       </c>
       <c r="B89">
         <f t="shared" si="7"/>
-        <v>3031160.3205609075</v>
+        <v>1192637.1972651451</v>
       </c>
       <c r="C89">
         <f t="shared" si="5"/>
-        <v>276951.64538095082</v>
+        <v>271031.89014767861</v>
       </c>
       <c r="D89">
         <f t="shared" si="8"/>
-        <v>5763598.8319361946</v>
+        <v>5918331.6584828747</v>
       </c>
       <c r="E89">
         <f t="shared" si="9"/>
-        <v>63081019.283945486</v>
+        <v>26042774.810789354</v>
       </c>
       <c r="F89">
         <f t="shared" si="6"/>
-        <v>266742108.20935985</v>
+        <v>104952073.35933277</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -4571,23 +4793,23 @@
       </c>
       <c r="B90">
         <f t="shared" si="7"/>
-        <v>3147506.8852891321</v>
+        <v>1235502.904666553</v>
       </c>
       <c r="C90">
         <f t="shared" si="5"/>
-        <v>287582.02092306019</v>
+        <v>280773.3049938383</v>
       </c>
       <c r="D90">
         <f t="shared" si="8"/>
-        <v>6051180.8528592549</v>
+        <v>6199104.9634767128</v>
       </c>
       <c r="E90">
         <f t="shared" si="9"/>
-        <v>66228526.169234619</v>
+        <v>27278277.715455908</v>
       </c>
       <c r="F90">
         <f t="shared" si="6"/>
-        <v>280128112.79073274</v>
+        <v>109959758.51532322</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -4596,23 +4818,23 @@
       </c>
       <c r="B91">
         <f t="shared" si="7"/>
-        <v>3266944.0602401705</v>
+        <v>1279404.4059847156</v>
       </c>
       <c r="C91">
         <f t="shared" si="5"/>
-        <v>298494.77994077571</v>
+        <v>290750.10842565104</v>
       </c>
       <c r="D91">
         <f t="shared" si="8"/>
-        <v>6349675.6328000305</v>
+        <v>6489855.0719023636</v>
       </c>
       <c r="E91">
         <f t="shared" si="9"/>
-        <v>69495470.229474783</v>
+        <v>28557682.121440623</v>
       </c>
       <c r="F91">
         <f t="shared" si="6"/>
-        <v>294024965.42161536</v>
+        <v>115146396.53862441</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -4621,23 +4843,23 @@
       </c>
       <c r="B92">
         <f t="shared" si="7"/>
-        <v>3389518.2328576325</v>
+        <v>1324354.8032504446</v>
       </c>
       <c r="C92">
         <f t="shared" si="5"/>
-        <v>309694.16077106219</v>
+        <v>300965.27793550416</v>
       </c>
       <c r="D92">
         <f t="shared" si="8"/>
-        <v>6659369.7935710931</v>
+        <v>6790820.3498378675</v>
       </c>
       <c r="E92">
         <f t="shared" si="9"/>
-        <v>72884988.462332413</v>
+        <v>29882036.924691066</v>
       </c>
       <c r="F92">
         <f t="shared" si="6"/>
-        <v>308446159.19004458</v>
+        <v>120516287.09579046</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -4646,23 +4868,23 @@
       </c>
       <c r="B93">
         <f t="shared" si="7"/>
-        <v>3515275.962714375</v>
+        <v>1370367.2167051504</v>
       </c>
       <c r="C93">
         <f t="shared" si="5"/>
-        <v>321184.41747802281</v>
+        <v>311421.79515422118</v>
       </c>
       <c r="D93">
         <f t="shared" si="8"/>
-        <v>6980554.2110491162</v>
+        <v>7102242.1449920889</v>
       </c>
       <c r="E93">
         <f t="shared" si="9"/>
-        <v>76400264.425046787</v>
+        <v>31252404.141396217</v>
       </c>
       <c r="F93">
         <f t="shared" si="6"/>
-        <v>323405388.56972247</v>
+        <v>126073783.93687384</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -4671,23 +4893,23 @@
       </c>
       <c r="B94">
         <f t="shared" si="7"/>
-        <v>3644263.9802490319</v>
+        <v>1417454.7846255894</v>
       </c>
       <c r="C94">
         <f t="shared" si="5"/>
-        <v>332969.81973745843</v>
+        <v>322122.64581123489</v>
       </c>
       <c r="D94">
         <f t="shared" si="8"/>
-        <v>7313524.0307865748</v>
+        <v>7424364.7908033235</v>
       </c>
       <c r="E94">
         <f t="shared" si="9"/>
-        <v>80044528.405295819</v>
+        <v>32669858.926021807</v>
       </c>
       <c r="F94">
         <f t="shared" si="6"/>
-        <v>338916550.16315997</v>
+        <v>131823294.97017981</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -4696,23 +4918,23 @@
       </c>
       <c r="B95">
         <f t="shared" si="7"/>
-        <v>3776529.185525523</v>
+        <v>1465630.663152206</v>
       </c>
       <c r="C95">
         <f t="shared" si="5"/>
-        <v>345054.652723526</v>
+        <v>333070.81969557755</v>
       </c>
       <c r="D95">
         <f t="shared" si="8"/>
-        <v>7658578.6835101005</v>
+        <v>7757435.6104989015</v>
       </c>
       <c r="E95">
         <f t="shared" si="9"/>
-        <v>83821057.590821341</v>
+        <v>34135489.58917401</v>
       </c>
       <c r="F95">
         <f t="shared" si="6"/>
-        <v>354993743.43939918</v>
+        <v>137769282.33630738</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -4721,23 +4943,23 @@
       </c>
       <c r="B96">
         <f t="shared" si="7"/>
-        <v>3912118.6470148927</v>
+        <v>1514908.026120946</v>
       </c>
       <c r="C96">
         <f t="shared" si="5"/>
-        <v>357443.21699743712</v>
+        <v>344269.31061765942</v>
       </c>
       <c r="D96">
         <f t="shared" si="8"/>
-        <v>8016021.9005075376</v>
+        <v>8101704.9211165607</v>
       </c>
       <c r="E96">
         <f t="shared" si="9"/>
-        <v>87733176.237836227</v>
+        <v>35650397.615294956</v>
       </c>
       <c r="F96">
         <f t="shared" si="6"/>
-        <v>371651271.46641481</v>
+        <v>143916262.48148987</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -4746,23 +4968,23 @@
       </c>
       <c r="B97">
         <f t="shared" si="7"/>
-        <v>4051079.6003986518</v>
+        <v>1565300.0648983978</v>
       </c>
       <c r="C97">
         <f t="shared" si="5"/>
-        <v>370139.82839812216</v>
+        <v>355721.11637180398</v>
       </c>
       <c r="D97">
         <f t="shared" si="8"/>
-        <v>8386161.7289056601</v>
+        <v>8457426.0374883655</v>
       </c>
       <c r="E97">
         <f t="shared" si="9"/>
-        <v>91784255.838234872</v>
+        <v>37215697.68019335</v>
       </c>
       <c r="F97">
         <f t="shared" si="6"/>
-        <v>388903641.63827056</v>
+        <v>150268806.23024619</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -4771,23 +4993,23 @@
       </c>
       <c r="B98">
         <f t="shared" si="7"/>
-        <v>4193459.4473932683</v>
+        <v>1616819.9882202211</v>
       </c>
       <c r="C98">
         <f t="shared" si="5"/>
-        <v>383148.81793482543</v>
+        <v>367429.23869953048</v>
       </c>
       <c r="D98">
         <f t="shared" si="8"/>
-        <v>8769310.5468404852</v>
+        <v>8824855.2761878967</v>
       </c>
       <c r="E98">
         <f t="shared" si="9"/>
-        <v>95977715.28562814</v>
+        <v>38832517.668413572</v>
       </c>
       <c r="F98">
         <f t="shared" si="6"/>
-        <v>406765566.39714706</v>
+        <v>156831538.85736144</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -4796,23 +5018,23 @@
       </c>
       <c r="B99">
         <f t="shared" si="7"/>
-        <v>4339305.7545950767</v>
+        <v>1669481.0220327165</v>
       </c>
       <c r="C99">
         <f t="shared" si="5"/>
-        <v>396474.5316815672</v>
+        <v>379396.68325354968</v>
       </c>
       <c r="D99">
         <f t="shared" si="8"/>
-        <v>9165785.0785220526</v>
+        <v>9204251.9594414458</v>
       </c>
       <c r="E99">
         <f t="shared" si="9"/>
-        <v>100317021.04022321</v>
+        <v>40501998.690446287</v>
       </c>
       <c r="F99">
         <f t="shared" si="6"/>
-        <v>425251963.9503175</v>
+        <v>163609140.15920621</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -4821,23 +5043,23 @@
       </c>
       <c r="B100">
         <f t="shared" si="7"/>
-        <v>4488666.2523449976</v>
+        <v>1723296.4093374568</v>
       </c>
       <c r="C100">
         <f t="shared" si="5"/>
-        <v>410121.33067341452</v>
+        <v>391626.45956245554</v>
       </c>
       <c r="D100">
         <f t="shared" si="8"/>
-        <v>9575906.4091954678</v>
+        <v>9595878.419003902</v>
       </c>
       <c r="E100">
         <f t="shared" si="9"/>
-        <v>104805687.29256821</v>
+        <v>42225295.099783741</v>
       </c>
       <c r="F100">
         <f t="shared" si="6"/>
-        <v>444377958.98215479</v>
+        <v>170606344.52440822</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -4846,23 +5068,23 @@
       </c>
       <c r="B101">
         <f t="shared" si="7"/>
-        <v>4641588.8336127773</v>
+        <v>1778279.4100389304</v>
       </c>
       <c r="C101">
         <f t="shared" si="5"/>
-        <v>424093.59080453706</v>
+        <v>404121.58099610178</v>
       </c>
       <c r="D101">
-        <f t="shared" si="8"/>
-        <v>10000000.000000006</v>
+        <f>D100+C101</f>
+        <v>10000000.000000004</v>
       </c>
       <c r="E101">
         <f t="shared" si="9"/>
-        <v>109447276.12618098</v>
+        <v>44003574.509822674</v>
       </c>
       <c r="F101">
         <f t="shared" si="6"/>
-        <v>464158883.3612777</v>
+        <v>177827941.00389305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tried to match GDP
</commit_message>
<xml_diff>
--- a/PPPConverter/Sources/TempCalc.xlsx
+++ b/PPPConverter/Sources/TempCalc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Draco\source\repos\dracoranger\PPPConverter\PPPConverter\Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4200A68-7F96-4945-B5B6-601F5C75081D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2C3C6A-3F92-4912-BCF0-AF34CCD723C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-7875" windowWidth="21840" windowHeight="38040" xr2:uid="{7CE1D539-8B48-47E8-809E-63922FA2B7F3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{7CE1D539-8B48-47E8-809E-63922FA2B7F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>Food</t>
   </si>
@@ -102,18 +102,75 @@
   <si>
     <t>Total Wealth (Assets, cash, etc)</t>
   </si>
+  <si>
+    <t>GDP</t>
+  </si>
+  <si>
+    <t>Agriculture</t>
+  </si>
+  <si>
+    <t>Utilities</t>
+  </si>
+  <si>
+    <t>Construction</t>
+  </si>
+  <si>
+    <t>Manufactured goods</t>
+  </si>
+  <si>
+    <t>Total GDP</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>Government</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>Professional services</t>
+  </si>
+  <si>
+    <t>Trade</t>
+  </si>
+  <si>
+    <t>Edu, Health, Social</t>
+  </si>
+  <si>
+    <t>Arts</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Mining</t>
+  </si>
+  <si>
+    <t>Information</t>
+  </si>
+  <si>
+    <t>Transportation and warehousing</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -136,8 +193,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1961,16 +2019,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D864C3B-E825-406D-92B0-B90D1A840648}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2130,36 +2191,36 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <f>B2*B7</f>
+        <f>ROUND(B2*B7,4)</f>
         <v>0.51990000000000003</v>
       </c>
       <c r="C6">
-        <f t="shared" ref="C6:I6" si="2">C2*C7</f>
-        <v>5.3750000000000006E-2</v>
+        <f t="shared" ref="C6:I6" si="2">ROUND(C2*C7,4)</f>
+        <v>5.3800000000000001E-2</v>
       </c>
       <c r="D6">
         <f t="shared" si="2"/>
-        <v>0.15537500000000001</v>
+        <v>0.15540000000000001</v>
       </c>
       <c r="E6">
         <f t="shared" si="2"/>
-        <v>8.2475000000000021E-2</v>
+        <v>8.2500000000000004E-2</v>
       </c>
       <c r="F6">
         <f t="shared" si="2"/>
-        <v>8.9249999999999996E-2</v>
+        <v>8.9300000000000004E-2</v>
       </c>
       <c r="G6">
         <f t="shared" si="2"/>
-        <v>7.7550000000000008E-2</v>
+        <v>7.7600000000000002E-2</v>
       </c>
       <c r="H6">
         <f t="shared" si="2"/>
-        <v>3.0175E-2</v>
+        <v>3.0200000000000001E-2</v>
       </c>
       <c r="I6">
         <f t="shared" si="2"/>
-        <v>3.0525000000000004E-2</v>
+        <v>3.0499999999999999E-2</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2201,20 +2262,20 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <f>B2*B9</f>
+        <f>ROUND(B2*B9,4)</f>
         <v>0.38979999999999998</v>
       </c>
       <c r="C8">
-        <f t="shared" ref="C8:I8" si="3">C2*C9</f>
-        <v>5.7500000000000009E-2</v>
+        <f t="shared" ref="C8:I8" si="3">ROUND(C2*C9,4)</f>
+        <v>5.7500000000000002E-2</v>
       </c>
       <c r="D8">
         <f t="shared" si="3"/>
-        <v>0.21074999999999999</v>
+        <v>0.21079999999999999</v>
       </c>
       <c r="E8">
         <f t="shared" si="3"/>
-        <v>6.4950000000000022E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="F8">
         <f t="shared" si="3"/>
@@ -2222,24 +2283,24 @@
       </c>
       <c r="G8">
         <f t="shared" si="3"/>
-        <v>5.510000000000001E-2</v>
+        <v>5.5100000000000003E-2</v>
       </c>
       <c r="H8">
         <f t="shared" si="3"/>
-        <v>5.9350000000000007E-2</v>
+        <v>5.9400000000000001E-2</v>
       </c>
       <c r="I8">
         <f t="shared" si="3"/>
-        <v>6.0049999999999999E-2</v>
+        <v>6.0100000000000001E-2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9">
-        <f t="shared" ref="B8:B11" si="4">B7-(1/4*($B$5-$B$13))</f>
+        <f t="shared" ref="B9:B11" si="4">B7-(1/4*($B$5-$B$13))</f>
         <v>3.007716049382716</v>
       </c>
       <c r="C9">
-        <f t="shared" ref="C8:D11" si="5">C7+(1/4*(C$13-C$5))</f>
+        <f t="shared" ref="C9:D11" si="5">C7+(1/4*(C$13-C$5))</f>
         <v>0.88461538461538469</v>
       </c>
       <c r="D9">
@@ -2247,15 +2308,15 @@
         <v>0.65552099533437014</v>
       </c>
       <c r="E9">
-        <f t="shared" ref="E8:E11" si="6">E7-(1/4*($E$5-$E$13))</f>
+        <f t="shared" ref="E9:E11" si="6">E7-(1/4*($E$5-$E$13))</f>
         <v>2.1722408026755859</v>
       </c>
       <c r="F9">
-        <f t="shared" ref="F8:F11" si="7">F7+(1/4*(F$13-F$5))</f>
+        <f t="shared" ref="F9:F11" si="7">F7+(1/4*(F$13-F$5))</f>
         <v>0.62077294685990347</v>
       </c>
       <c r="G9">
-        <f t="shared" ref="G8:G11" si="8">G7-(1/4*($G$5-$G$13))</f>
+        <f t="shared" ref="G9:G11" si="8">G7-(1/4*($G$5-$G$13))</f>
         <v>5.4019607843137258</v>
       </c>
       <c r="H9">
@@ -2272,36 +2333,36 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <f>B2*B11</f>
-        <v>0.25969999999999993</v>
+        <f>ROUND(B2*B11,4)</f>
+        <v>0.25969999999999999</v>
       </c>
       <c r="C10">
-        <f t="shared" ref="C10:I10" si="10">C2*C11</f>
-        <v>6.1250000000000006E-2</v>
+        <f t="shared" ref="C10:I10" si="10">ROUND(C2*C11,4)</f>
+        <v>6.13E-2</v>
       </c>
       <c r="D10">
         <f t="shared" si="10"/>
-        <v>0.266125</v>
+        <v>0.2661</v>
       </c>
       <c r="E10">
         <f t="shared" si="10"/>
-        <v>4.7425000000000016E-2</v>
+        <v>4.7399999999999998E-2</v>
       </c>
       <c r="F10">
         <f t="shared" si="10"/>
-        <v>0.16775000000000001</v>
+        <v>0.1678</v>
       </c>
       <c r="G10">
         <f t="shared" si="10"/>
-        <v>3.2650000000000005E-2</v>
+        <v>3.27E-2</v>
       </c>
       <c r="H10">
         <f t="shared" si="10"/>
-        <v>8.8525000000000006E-2</v>
+        <v>8.8499999999999995E-2</v>
       </c>
       <c r="I10">
         <f t="shared" si="10"/>
-        <v>8.9575000000000002E-2</v>
+        <v>8.9599999999999999E-2</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2343,11 +2404,11 @@
         <v>8</v>
       </c>
       <c r="B12">
-        <f>B2*B13</f>
+        <f>ROUND(B2*B13,4)</f>
         <v>0.12959999999999999</v>
       </c>
       <c r="C12">
-        <f t="shared" ref="C12:I12" si="12">C2*C13</f>
+        <f t="shared" ref="C12:I12" si="12">ROUND(C2*C13,4)</f>
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="D12">
@@ -2472,7 +2533,7 @@
         <v>1.2479009235936189</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -2480,7 +2541,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>0.13</v>
       </c>
@@ -2506,8 +2567,298 @@
         <v>0.14862500000000001</v>
       </c>
     </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" t="s">
+        <v>32</v>
+      </c>
+      <c r="H25" t="s">
+        <v>34</v>
+      </c>
+      <c r="I25" t="s">
+        <v>33</v>
+      </c>
+      <c r="J25" t="s">
+        <v>36</v>
+      </c>
+      <c r="K25" t="s">
+        <v>37</v>
+      </c>
+      <c r="L25" t="s">
+        <v>38</v>
+      </c>
+      <c r="M25" t="s">
+        <v>39</v>
+      </c>
+      <c r="N25" t="s">
+        <v>40</v>
+      </c>
+      <c r="O25" t="s">
+        <v>41</v>
+      </c>
+      <c r="P25" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1">
+        <v>175.8</v>
+      </c>
+      <c r="C26">
+        <v>336.9</v>
+      </c>
+      <c r="D26">
+        <v>897.6</v>
+      </c>
+      <c r="E26">
+        <v>2418.6</v>
+      </c>
+      <c r="F26">
+        <v>2269.1999999999998</v>
+      </c>
+      <c r="G26">
+        <v>2645.7</v>
+      </c>
+      <c r="H26">
+        <v>2673.6</v>
+      </c>
+      <c r="I26">
+        <v>4660.2</v>
+      </c>
+      <c r="J26">
+        <v>1807.5</v>
+      </c>
+      <c r="K26">
+        <v>679.7</v>
+      </c>
+      <c r="L26">
+        <v>421.9</v>
+      </c>
+      <c r="M26">
+        <v>336.9</v>
+      </c>
+      <c r="N26">
+        <v>1161.4000000000001</v>
+      </c>
+      <c r="O26">
+        <v>595.9</v>
+      </c>
+      <c r="P26">
+        <v>20936.599999999999</v>
+      </c>
+      <c r="Q26">
+        <f>P26-SUM(B26:O26)</f>
+        <v>-144.30000000000655</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <f>B26/$P$26</f>
+        <v>8.3967788466131101E-3</v>
+      </c>
+      <c r="C27">
+        <f>C26/$P$26</f>
+        <v>1.6091437960318294E-2</v>
+      </c>
+      <c r="D27">
+        <f>D26/$P$26</f>
+        <v>4.287229062980618E-2</v>
+      </c>
+      <c r="E27">
+        <f>E26/$P$26</f>
+        <v>0.11552018952456464</v>
+      </c>
+      <c r="F27">
+        <f>F26/$P$26</f>
+        <v>0.10838436040235759</v>
+      </c>
+      <c r="G27">
+        <f>G26/$P$26</f>
+        <v>0.12636722294928499</v>
+      </c>
+      <c r="H27">
+        <f>H26/$P$26</f>
+        <v>0.12769981754439594</v>
+      </c>
+      <c r="I27">
+        <f>I26/$P$26</f>
+        <v>0.22258628430595226</v>
+      </c>
+      <c r="J27">
+        <f>J26/$P$26</f>
+        <v>8.6332069199392458E-2</v>
+      </c>
+      <c r="K27">
+        <f t="shared" ref="K27:O27" si="21">K26/$P$26</f>
+        <v>3.2464679078742495E-2</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="21"/>
+        <v>2.0151313966928729E-2</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="21"/>
+        <v>1.6091437960318294E-2</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="21"/>
+        <v>5.5472235224439503E-2</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="21"/>
+        <v>2.8462118968695969E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <f>ROUND(B27,3)</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C28">
+        <f t="shared" ref="C28:O28" si="22">ROUND(C27,3)</f>
+        <v>1.6E-2</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="22"/>
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="22"/>
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="22"/>
+        <v>0.108</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="22"/>
+        <v>0.126</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="22"/>
+        <v>0.128</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="22"/>
+        <v>0.223</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="22"/>
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="22"/>
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="22"/>
+        <v>0.02</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="22"/>
+        <v>1.6E-2</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="22"/>
+        <v>5.5E-2</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="22"/>
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="Q28">
+        <f>1-SUM(B28:O28)</f>
+        <v>-4.9999999999998934E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <f>ROUND(B28*(1+$Q$28),3)</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C29">
+        <f t="shared" ref="C29:O29" si="23">ROUND(C28*(1+$Q$28),3)</f>
+        <v>1.6E-2</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="23"/>
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="23"/>
+        <v>0.115</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="23"/>
+        <v>0.107</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="23"/>
+        <v>0.125</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="23"/>
+        <v>0.127</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="23"/>
+        <v>0.222</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="23"/>
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="23"/>
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="23"/>
+        <v>0.02</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="23"/>
+        <v>1.6E-2</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="23"/>
+        <v>5.5E-2</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="23"/>
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="Q29">
+        <f>SUM(B29:O29)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4250,7 +4601,7 @@
         <v>115610.1066437165</v>
       </c>
       <c r="D68">
-        <f t="shared" ref="D68:D101" si="8">D67+C68</f>
+        <f t="shared" ref="D68:D100" si="8">D67+C68</f>
         <v>1936042.8050735693</v>
       </c>
       <c r="E68">

</xml_diff>